<commit_message>
2º Commit de correções conf. feedback Professor
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="46">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -54,32 +54,117 @@
     <t>Criar Tela de  Localização de Veículos</t>
   </si>
   <si>
-    <t>Realizar Análise de Sistema</t>
-  </si>
-  <si>
-    <t>Requisitos do Sistema de Rastreamento</t>
-  </si>
-  <si>
-    <t>Criar Projeto do Sistema de Rastreamento</t>
-  </si>
-  <si>
-    <t>Implementação do Sistema de Rastreamento</t>
-  </si>
-  <si>
     <t>Criar tela de Login do Sistema de Rastreamento</t>
   </si>
   <si>
     <t>Realizar Testes Tela Localização de veículos</t>
   </si>
   <si>
-    <t>Realizar Testes Tela Login no Sistema de Ratsreamento</t>
+    <t>Abrir uma conta no GitHub</t>
+  </si>
+  <si>
+    <t>Concluído</t>
+  </si>
+  <si>
+    <t>https://github.com</t>
+  </si>
+  <si>
+    <t>Configurar o GitHub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valter </t>
+  </si>
+  <si>
+    <t>0.30</t>
+  </si>
+  <si>
+    <t>Criar o Documento de Visão</t>
+  </si>
+  <si>
+    <t>http://meuprojeto.net/processo/</t>
+  </si>
+  <si>
+    <t>Criar o Documento Plano de Projeto</t>
+  </si>
+  <si>
+    <t>Criar o Documento Lista de Riscos</t>
+  </si>
+  <si>
+    <t>Criar o Documento Lista de Itens de Trabalho</t>
+  </si>
+  <si>
+    <t>Criar o Documento Especificação do Caso de Uso</t>
+  </si>
+  <si>
+    <t>Criar o Documento Plano de Iteração</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste</t>
+  </si>
+  <si>
+    <t>média'</t>
+  </si>
+  <si>
+    <t>http://www.uml.org/</t>
+  </si>
+  <si>
+    <t>Atualizar o Documento de Visão</t>
+  </si>
+  <si>
+    <t>Atualizar o Documento Plano de Projeto</t>
+  </si>
+  <si>
+    <t>Atualizar o Documento Lista de Riscos</t>
+  </si>
+  <si>
+    <t>Atualizar o Documento Lista de Itens de Trabalho</t>
+  </si>
+  <si>
+    <t>Atualizar o Documento Especificação do Caso de Uso</t>
+  </si>
+  <si>
+    <t>Atualizar o Documento Plano de Iteração</t>
+  </si>
+  <si>
+    <t>Atualizar a  Planilha de Caso de Teste</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_1</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_2</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>Configuração de pastas no GITHUB conforme feedback</t>
+  </si>
+  <si>
+    <t>1.2</t>
+  </si>
+  <si>
+    <t>Realizar Testes Tela Login no Sistema de Rastreamento</t>
+  </si>
+  <si>
+    <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades Tela Localização de Veículos</t>
+  </si>
+  <si>
+    <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades Tela Logar no Sistema</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="169" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -98,6 +183,29 @@
     <font>
       <u/>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0070C0"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -146,10 +254,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -158,13 +269,32 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
+    <cellStyle name="Separador de milhares" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -456,10 +586,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -468,8 +598,8 @@
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.7109375" customWidth="1"/>
-    <col min="9" max="9" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="9" max="9" width="56" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25">
@@ -503,171 +633,633 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>180</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="6">
+        <v>120</v>
+      </c>
+      <c r="H4">
+        <v>145</v>
+      </c>
+      <c r="I4" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>160</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="6">
+        <v>240</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="I5" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6">
+        <v>140</v>
+      </c>
+      <c r="D6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="6">
+        <v>82</v>
+      </c>
+      <c r="H6">
+        <v>70</v>
+      </c>
+      <c r="I6" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>160</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="6">
+        <v>110</v>
+      </c>
+      <c r="H7">
+        <v>90</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>130</v>
+      </c>
+      <c r="D8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="6">
+        <v>65</v>
+      </c>
+      <c r="H8">
+        <v>70</v>
+      </c>
+      <c r="I8" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>165</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="6">
+        <v>82</v>
+      </c>
+      <c r="H9">
+        <v>85</v>
+      </c>
+      <c r="I9" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>110</v>
+      </c>
+      <c r="D10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="6">
+        <v>62</v>
+      </c>
+      <c r="H10">
+        <v>65</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>50</v>
+      </c>
+      <c r="D11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="25.5">
+      <c r="A12" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12">
+        <v>80</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="6">
+        <v>180</v>
+      </c>
+      <c r="H12">
+        <v>160</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>40</v>
+      </c>
+      <c r="D13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="6">
+        <v>72</v>
+      </c>
+      <c r="H13" s="8">
+        <v>82</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>20</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="6">
+        <v>160</v>
+      </c>
+      <c r="H14" s="8">
+        <v>150</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
+        <v>60</v>
+      </c>
+      <c r="D15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>18</v>
+      </c>
+      <c r="G15" s="6">
+        <v>120</v>
+      </c>
+      <c r="H15" s="8">
+        <v>110</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G16" s="6">
+        <v>160</v>
+      </c>
+      <c r="H16" s="8">
+        <v>160</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" t="s">
+        <v>18</v>
+      </c>
+      <c r="G17" s="6">
+        <v>120</v>
+      </c>
+      <c r="H17">
+        <v>135</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="F18" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="6">
         <v>240</v>
       </c>
-      <c r="H2" s="6">
-        <v>1.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3">
-        <v>15</v>
-      </c>
-      <c r="D3" s="6">
-        <v>1</v>
-      </c>
-      <c r="G3">
-        <v>360</v>
-      </c>
-      <c r="H3" s="6">
-        <v>2.1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
+      <c r="H18">
+        <v>210</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
         <v>40</v>
       </c>
-      <c r="D4" s="6">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>480</v>
-      </c>
-      <c r="H4" s="6">
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
-      <c r="A5" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5">
-        <v>20</v>
-      </c>
-      <c r="D5" s="6">
-        <v>0.8</v>
-      </c>
-      <c r="G5">
-        <v>530</v>
-      </c>
-      <c r="H5" s="6">
-        <v>2.2000000000000002</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6">
+      <c r="D19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="6">
+        <v>82</v>
+      </c>
+      <c r="H19">
+        <v>90</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
+      <c r="A20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20">
+        <v>60</v>
+      </c>
+      <c r="D20" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="6">
+        <v>110</v>
+      </c>
+      <c r="H20">
+        <v>100</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
         <v>40</v>
       </c>
-      <c r="D6" s="6">
-        <v>1</v>
-      </c>
-      <c r="G6">
-        <v>72</v>
-      </c>
-      <c r="H6" s="6">
-        <v>0.83</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7" s="6">
-        <v>1</v>
-      </c>
-      <c r="G7">
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" t="s">
+        <v>18</v>
+      </c>
+      <c r="G21" s="6">
+        <v>65</v>
+      </c>
+      <c r="H21">
+        <v>35</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
+      <c r="A22" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22">
+        <v>80</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.95</v>
+      </c>
+      <c r="F22" t="s">
+        <v>18</v>
+      </c>
+      <c r="G22" s="6">
+        <v>82</v>
+      </c>
+      <c r="H22">
+        <v>40</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
+      <c r="A23" t="s">
+        <v>36</v>
+      </c>
+      <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23">
+        <v>60</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.85</v>
+      </c>
+      <c r="F23" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="6">
+        <v>62</v>
+      </c>
+      <c r="H23">
+        <v>25</v>
+      </c>
+      <c r="I23" s="11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="25.5">
+      <c r="A24" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24">
+        <v>80</v>
+      </c>
+      <c r="D24" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>18</v>
+      </c>
+      <c r="G24" s="6">
+        <v>180</v>
+      </c>
+      <c r="H24">
         <v>160</v>
       </c>
-      <c r="H7" s="6">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8">
-        <v>60</v>
-      </c>
-      <c r="D8" s="6">
-        <v>1</v>
-      </c>
-      <c r="G8">
-        <v>120</v>
-      </c>
-      <c r="H8" s="6">
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-      <c r="D9" s="6">
-        <v>1</v>
-      </c>
-      <c r="G9">
-        <v>160</v>
-      </c>
-      <c r="H9" s="6">
-        <v>0.52</v>
-      </c>
-    </row>
-    <row r="23" spans="6:6">
-      <c r="F23" s="7"/>
+      <c r="I24" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="6:6">
+      <c r="F38" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="I4" r:id="rId1"/>
+    <hyperlink ref="I5" r:id="rId2"/>
+    <hyperlink ref="I6" r:id="rId3"/>
+    <hyperlink ref="I7" r:id="rId4"/>
+    <hyperlink ref="I8" r:id="rId5"/>
+    <hyperlink ref="I9" r:id="rId6"/>
+    <hyperlink ref="I12" r:id="rId7"/>
+    <hyperlink ref="I10" r:id="rId8"/>
+    <hyperlink ref="I13" r:id="rId9"/>
+    <hyperlink ref="I14:I23" r:id="rId10" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I14" r:id="rId11"/>
+    <hyperlink ref="I15" r:id="rId12"/>
+    <hyperlink ref="I16" r:id="rId13"/>
+    <hyperlink ref="I17" r:id="rId14"/>
+    <hyperlink ref="I18" r:id="rId15"/>
+    <hyperlink ref="I19" r:id="rId16"/>
+    <hyperlink ref="I20" r:id="rId17"/>
+    <hyperlink ref="I21" r:id="rId18"/>
+    <hyperlink ref="I22" r:id="rId19"/>
+    <hyperlink ref="I23" r:id="rId20"/>
+    <hyperlink ref="I11" r:id="rId21"/>
+    <hyperlink ref="I24" r:id="rId22" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+  </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId23"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atualização diversas e algumas correções
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="49">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -51,15 +51,6 @@
     <t>Média</t>
   </si>
   <si>
-    <t>Criar Tela de  Localização de Veículos</t>
-  </si>
-  <si>
-    <t>Criar tela de Login do Sistema de Rastreamento</t>
-  </si>
-  <si>
-    <t>Realizar Testes Tela Localização de veículos</t>
-  </si>
-  <si>
     <t>Abrir uma conta no GitHub</t>
   </si>
   <si>
@@ -99,12 +90,6 @@
     <t>Criar o Documento Plano de Iteração</t>
   </si>
   <si>
-    <t>Criar Planilha de Caso de Teste</t>
-  </si>
-  <si>
-    <t>média'</t>
-  </si>
-  <si>
     <t>http://www.uml.org/</t>
   </si>
   <si>
@@ -132,9 +117,6 @@
     <t>https://github.com/valtervasconcelos/Projeto_de_Software_1</t>
   </si>
   <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_2</t>
-  </si>
-  <si>
     <t>1.5</t>
   </si>
   <si>
@@ -147,13 +129,40 @@
     <t>1.2</t>
   </si>
   <si>
-    <t>Realizar Testes Tela Login no Sistema de Rastreamento</t>
-  </si>
-  <si>
-    <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades Tela Localização de Veículos</t>
-  </si>
-  <si>
     <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades Tela Logar no Sistema</t>
+  </si>
+  <si>
+    <t>Planejar Iterações Logar no Sistema</t>
+  </si>
+  <si>
+    <t>Especificar o Caso de Uso Logar no Sistema</t>
+  </si>
+  <si>
+    <t>Criar tela Logar no Sistema</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Logar no Sistema</t>
+  </si>
+  <si>
+    <t>Criar Tela Localizar Veículo</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Localizar Veículo</t>
+  </si>
+  <si>
+    <t>Realizar Análise do Sistema de Rastreamento</t>
+  </si>
+  <si>
+    <t>Planejar Iterações Localizar Veículo</t>
+  </si>
+  <si>
+    <t>Especificar o Caso de Uso Localizar Veículo</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Logar no Sistema</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Localizar Veículo</t>
   </si>
 </sst>
 </file>
@@ -260,7 +269,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -289,6 +298,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -586,10 +596,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I38"/>
+  <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -633,7 +643,7 @@
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
@@ -642,24 +652,24 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="H2">
         <v>0.5</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -668,102 +678,102 @@
         <v>20</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6">
+        <v>32</v>
+      </c>
+      <c r="H4" s="6">
+        <v>48</v>
+      </c>
+      <c r="I4" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I3" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>180</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="6">
-        <v>120</v>
-      </c>
-      <c r="H4">
-        <v>145</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6">
+        <v>82</v>
+      </c>
+      <c r="H5">
+        <v>85</v>
+      </c>
+      <c r="I5" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="G5" s="6">
-        <v>240</v>
-      </c>
-      <c r="H5">
-        <v>200</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
       </c>
       <c r="C6">
-        <v>140</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="6">
+        <v>120</v>
+      </c>
+      <c r="H6">
+        <v>145</v>
+      </c>
+      <c r="I6" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="G6" s="6">
-        <v>82</v>
-      </c>
-      <c r="H6">
-        <v>70</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -772,102 +782,102 @@
         <v>160</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" s="6">
+        <v>240</v>
+      </c>
+      <c r="H7">
+        <v>200</v>
+      </c>
+      <c r="I7" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="G7" s="6">
-        <v>110</v>
-      </c>
-      <c r="H7">
-        <v>90</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
       </c>
       <c r="C8">
-        <v>130</v>
+        <v>140</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G8" s="6">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="H8">
         <v>70</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
       <c r="C9">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="6">
+        <v>110</v>
+      </c>
+      <c r="H9">
+        <v>90</v>
+      </c>
+      <c r="I9" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="G9" s="6">
-        <v>82</v>
-      </c>
-      <c r="H9">
-        <v>85</v>
-      </c>
-      <c r="I9" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>110</v>
+        <v>130</v>
       </c>
       <c r="D10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="6">
+        <v>65</v>
+      </c>
+      <c r="H10">
+        <v>70</v>
+      </c>
+      <c r="I10" s="13" t="s">
         <v>18</v>
-      </c>
-      <c r="G10" s="6">
-        <v>62</v>
-      </c>
-      <c r="H10">
-        <v>65</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -876,36 +886,36 @@
         <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G11" s="6">
         <v>2</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="I11" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="25.5">
       <c r="A12" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="B12" t="s">
-        <v>28</v>
+        <v>37</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>10</v>
       </c>
       <c r="C12">
-        <v>80</v>
+        <v>220</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G12" s="6">
         <v>180</v>
@@ -914,194 +924,194 @@
         <v>160</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="4" t="s">
-        <v>12</v>
+      <c r="A13" s="16" t="s">
+        <v>38</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13">
+        <v>80</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6">
+        <v>120</v>
+      </c>
+      <c r="H13">
+        <v>135</v>
+      </c>
+      <c r="I13" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="6">
+        <v>240</v>
+      </c>
+      <c r="H14">
+        <v>210</v>
+      </c>
+      <c r="I14" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" t="s">
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6">
+        <v>82</v>
+      </c>
+      <c r="H15">
+        <v>90</v>
+      </c>
+      <c r="I15" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16">
+        <v>60</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6">
+        <v>110</v>
+      </c>
+      <c r="H16">
+        <v>100</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>40</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6">
+        <v>72</v>
+      </c>
+      <c r="H17" s="8">
+        <v>82</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>110</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="6">
+        <v>62</v>
+      </c>
+      <c r="H18">
+        <v>65</v>
+      </c>
+      <c r="I18" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G13" s="6">
-        <v>72</v>
-      </c>
-      <c r="H13" s="8">
-        <v>82</v>
-      </c>
-      <c r="I13" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" t="s">
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B19" t="s">
         <v>10</v>
       </c>
-      <c r="C14">
+      <c r="C19">
         <v>20</v>
       </c>
-      <c r="D14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G14" s="6">
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6">
         <v>160</v>
       </c>
-      <c r="H14" s="8">
+      <c r="H19" s="8">
         <v>150</v>
       </c>
-      <c r="I14" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15">
-        <v>60</v>
-      </c>
-      <c r="D15" t="s">
-        <v>15</v>
-      </c>
-      <c r="F15" t="s">
-        <v>18</v>
-      </c>
-      <c r="G15" s="6">
-        <v>120</v>
-      </c>
-      <c r="H15" s="8">
-        <v>110</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16">
-        <v>20</v>
-      </c>
-      <c r="D16" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="6">
-        <v>160</v>
-      </c>
-      <c r="H16" s="8">
-        <v>160</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17">
-        <v>80</v>
-      </c>
-      <c r="D17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" t="s">
-        <v>18</v>
-      </c>
-      <c r="G17" s="6">
-        <v>120</v>
-      </c>
-      <c r="H17">
-        <v>135</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>80</v>
-      </c>
-      <c r="D18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>18</v>
-      </c>
-      <c r="G18" s="6">
-        <v>240</v>
-      </c>
-      <c r="H18">
-        <v>210</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" t="s">
-        <v>32</v>
-      </c>
-      <c r="B19" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19">
-        <v>40</v>
-      </c>
-      <c r="D19" t="s">
-        <v>15</v>
-      </c>
-      <c r="F19" t="s">
-        <v>18</v>
-      </c>
-      <c r="G19" s="6">
-        <v>82</v>
-      </c>
-      <c r="H19">
-        <v>90</v>
-      </c>
       <c r="I19" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" t="s">
-        <v>33</v>
+      <c r="A20" s="4" t="s">
+        <v>42</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
@@ -1110,156 +1120,298 @@
         <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="6">
+        <v>120</v>
+      </c>
+      <c r="H20" s="8">
+        <v>110</v>
+      </c>
+      <c r="I20" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
+      <c r="A21" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21">
+        <v>110</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="6">
+        <v>62</v>
+      </c>
+      <c r="H21">
+        <v>65</v>
+      </c>
+      <c r="I21" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="G20" s="6">
-        <v>110</v>
-      </c>
-      <c r="H20">
-        <v>100</v>
-      </c>
-      <c r="I20" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" t="s">
-        <v>34</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>40</v>
-      </c>
-      <c r="D21" t="s">
-        <v>15</v>
-      </c>
-      <c r="F21" t="s">
-        <v>18</v>
-      </c>
-      <c r="G21" s="6">
-        <v>65</v>
-      </c>
-      <c r="H21">
-        <v>35</v>
-      </c>
-      <c r="I21" s="11" t="s">
-        <v>37</v>
-      </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" t="s">
-        <v>35</v>
+      <c r="A22" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C22">
-        <v>80</v>
-      </c>
-      <c r="D22" s="10">
-        <v>0.95</v>
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>12</v>
       </c>
       <c r="F22" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G22" s="6">
-        <v>82</v>
-      </c>
-      <c r="H22">
-        <v>40</v>
+        <v>160</v>
+      </c>
+      <c r="H22" s="8">
+        <v>150</v>
       </c>
       <c r="I22" s="11" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="C23">
-        <v>60</v>
-      </c>
-      <c r="D23" s="9">
-        <v>0.85</v>
+        <v>80</v>
+      </c>
+      <c r="D23" t="s">
+        <v>12</v>
       </c>
       <c r="F23" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G23" s="6">
-        <v>62</v>
+        <v>120</v>
       </c>
       <c r="H23">
-        <v>25</v>
+        <v>135</v>
       </c>
       <c r="I23" s="11" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="25.5">
-      <c r="A24" s="14" t="s">
-        <v>44</v>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
+      <c r="A24" t="s">
+        <v>26</v>
       </c>
       <c r="B24" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C24">
         <v>80</v>
       </c>
-      <c r="D24" s="7">
-        <v>0.9</v>
+      <c r="D24" t="s">
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G24" s="6">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="H24">
-        <v>160</v>
+        <v>210</v>
       </c>
       <c r="I24" s="11" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="38" spans="6:6">
-      <c r="F38" s="5"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>9</v>
+      </c>
+      <c r="C25">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="6">
+        <v>82</v>
+      </c>
+      <c r="H25">
+        <v>90</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26">
+        <v>60</v>
+      </c>
+      <c r="D26" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="6">
+        <v>110</v>
+      </c>
+      <c r="H26">
+        <v>100</v>
+      </c>
+      <c r="I26" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="6">
+        <v>65</v>
+      </c>
+      <c r="H27">
+        <v>35</v>
+      </c>
+      <c r="I27" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C28">
+        <v>80</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="6">
+        <v>82</v>
+      </c>
+      <c r="H28">
+        <v>40</v>
+      </c>
+      <c r="I28" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" t="s">
+        <v>34</v>
+      </c>
+      <c r="C29">
+        <v>60</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F29" t="s">
+        <v>15</v>
+      </c>
+      <c r="G29" s="6">
+        <v>62</v>
+      </c>
+      <c r="H29">
+        <v>25</v>
+      </c>
+      <c r="I29" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
+      <c r="A30" s="14"/>
+      <c r="D30" s="7"/>
+      <c r="G30" s="6"/>
+      <c r="I30" s="11"/>
+    </row>
+    <row r="44" spans="6:6">
+      <c r="F44" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="I4" r:id="rId1"/>
-    <hyperlink ref="I5" r:id="rId2"/>
-    <hyperlink ref="I6" r:id="rId3"/>
-    <hyperlink ref="I7" r:id="rId4"/>
-    <hyperlink ref="I8" r:id="rId5"/>
-    <hyperlink ref="I9" r:id="rId6"/>
+    <hyperlink ref="I6" r:id="rId1"/>
+    <hyperlink ref="I7" r:id="rId2"/>
+    <hyperlink ref="I8" r:id="rId3"/>
+    <hyperlink ref="I9" r:id="rId4"/>
+    <hyperlink ref="I10" r:id="rId5"/>
+    <hyperlink ref="I5" r:id="rId6"/>
     <hyperlink ref="I12" r:id="rId7"/>
-    <hyperlink ref="I10" r:id="rId8"/>
-    <hyperlink ref="I13" r:id="rId9"/>
-    <hyperlink ref="I14:I23" r:id="rId10" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I14" r:id="rId11"/>
-    <hyperlink ref="I15" r:id="rId12"/>
-    <hyperlink ref="I16" r:id="rId13"/>
-    <hyperlink ref="I17" r:id="rId14"/>
-    <hyperlink ref="I18" r:id="rId15"/>
-    <hyperlink ref="I19" r:id="rId16"/>
-    <hyperlink ref="I20" r:id="rId17"/>
-    <hyperlink ref="I21" r:id="rId18"/>
-    <hyperlink ref="I22" r:id="rId19"/>
-    <hyperlink ref="I23" r:id="rId20"/>
-    <hyperlink ref="I11" r:id="rId21"/>
-    <hyperlink ref="I24" r:id="rId22" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I17" r:id="rId8"/>
+    <hyperlink ref="I19:I29" r:id="rId9" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I19" r:id="rId10"/>
+    <hyperlink ref="I20" r:id="rId11"/>
+    <hyperlink ref="I23" r:id="rId12"/>
+    <hyperlink ref="I24" r:id="rId13"/>
+    <hyperlink ref="I25" r:id="rId14"/>
+    <hyperlink ref="I26" r:id="rId15"/>
+    <hyperlink ref="I27" r:id="rId16"/>
+    <hyperlink ref="I28" r:id="rId17"/>
+    <hyperlink ref="I29" r:id="rId18"/>
+    <hyperlink ref="I11" r:id="rId19"/>
+    <hyperlink ref="I18" r:id="rId20"/>
+    <hyperlink ref="I22" r:id="rId21"/>
+    <hyperlink ref="I21" r:id="rId22"/>
+    <hyperlink ref="I13:I16" r:id="rId23" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I13" r:id="rId24"/>
+    <hyperlink ref="I14" r:id="rId25"/>
+    <hyperlink ref="I15" r:id="rId26"/>
+    <hyperlink ref="I16" r:id="rId27"/>
+    <hyperlink ref="I4" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId23"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId29"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Correções para início de Projeto de Software II
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="51">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>Criar Planilha de Caso de Teste Localizar Veículo</t>
+  </si>
+  <si>
+    <t>Corrigir todos os documentos para o início de GPSII</t>
+  </si>
+  <si>
+    <t>0.5%</t>
   </si>
 </sst>
 </file>
@@ -599,7 +605,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1370,10 +1376,30 @@
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="14"/>
-      <c r="D30" s="7"/>
-      <c r="G30" s="6"/>
-      <c r="I30" s="11"/>
+      <c r="A30" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" t="s">
+        <v>9</v>
+      </c>
+      <c r="C30">
+        <v>100</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F30" t="s">
+        <v>15</v>
+      </c>
+      <c r="G30" s="6">
+        <v>6</v>
+      </c>
+      <c r="H30">
+        <v>0.5</v>
+      </c>
+      <c r="I30" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="44" spans="6:6">
       <c r="F44" s="5"/>
@@ -1409,9 +1435,10 @@
     <hyperlink ref="I15" r:id="rId26"/>
     <hyperlink ref="I16" r:id="rId27"/>
     <hyperlink ref="I4" r:id="rId28"/>
+    <hyperlink ref="I30" r:id="rId29"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId29"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId30"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Unificação dos Planos de Iteração em apenas E1
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -165,10 +165,10 @@
     <t>Criar Planilha de Caso de Teste Localizar Veículo</t>
   </si>
   <si>
-    <t>Corrigir todos os documentos para o início de GPSII</t>
-  </si>
-  <si>
     <t>0.5%</t>
+  </si>
+  <si>
+    <t>Corrigir todos os documentos para o início de PSWII</t>
   </si>
 </sst>
 </file>
@@ -605,7 +605,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1377,7 +1377,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="14" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
@@ -1386,7 +1386,7 @@
         <v>100</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Atualizar Lista de Ítens de Trabalho
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="50">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>Criar Planilha de Caso de Teste Localizar Veículo</t>
-  </si>
-  <si>
-    <t>0.5%</t>
   </si>
   <si>
     <t>Corrigir todos os documentos para o início de PSWII</t>
@@ -605,7 +602,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1377,7 +1374,7 @@
     </row>
     <row r="30" spans="1:9">
       <c r="A30" s="14" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
@@ -1385,8 +1382,8 @@
       <c r="C30">
         <v>100</v>
       </c>
-      <c r="D30" s="7" t="s">
-        <v>49</v>
+      <c r="D30" s="7">
+        <v>0.2</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -1395,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="H30">
-        <v>0.5</v>
+        <v>1.3</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Continuação de Correções para Inínio PSWII
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -602,7 +602,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I31" sqref="I31"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1383,7 +1383,7 @@
         <v>100</v>
       </c>
       <c r="D30" s="7">
-        <v>0.2</v>
+        <v>0.35</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -1392,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="H30">
-        <v>1.3</v>
+        <v>2.5</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Finalização de todas as correções em E1
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="50">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -602,7 +602,7 @@
   <dimension ref="A1:I44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+      <selection activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1382,8 +1382,8 @@
       <c r="C30">
         <v>100</v>
       </c>
-      <c r="D30" s="7">
-        <v>0.45</v>
+      <c r="D30" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="F30" t="s">
         <v>15</v>
@@ -1392,7 +1392,7 @@
         <v>6</v>
       </c>
       <c r="H30">
-        <v>3.5</v>
+        <v>4.5</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Criar Iteração E2 entre outros documentos
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="62">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -132,9 +132,6 @@
     <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades Tela Logar no Sistema</t>
   </si>
   <si>
-    <t>Planejar Iterações Logar no Sistema</t>
-  </si>
-  <si>
     <t>Especificar o Caso de Uso Logar no Sistema</t>
   </si>
   <si>
@@ -153,9 +150,6 @@
     <t>Realizar Análise do Sistema de Rastreamento</t>
   </si>
   <si>
-    <t>Planejar Iterações Localizar Veículo</t>
-  </si>
-  <si>
     <t>Especificar o Caso de Uso Localizar Veículo</t>
   </si>
   <si>
@@ -166,6 +160,48 @@
   </si>
   <si>
     <t>Corrigir todos os documentos para o início de PSWII</t>
+  </si>
+  <si>
+    <t>Criar Iteração E2</t>
+  </si>
+  <si>
+    <t>Valter/Edson</t>
+  </si>
+  <si>
+    <t>Criar Iteração E1</t>
+  </si>
+  <si>
+    <t>Criar tela Alterar Senha Gerência</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Alterar Senha Gerência</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Alterar Senha Gerência</t>
+  </si>
+  <si>
+    <t>Especificar o Caso de Uso Alterar Senha Gerência</t>
+  </si>
+  <si>
+    <t>Incompleto</t>
+  </si>
+  <si>
+    <t>9.20</t>
+  </si>
+  <si>
+    <t>0.20</t>
+  </si>
+  <si>
+    <t>0.10</t>
+  </si>
+  <si>
+    <t>0.15</t>
+  </si>
+  <si>
+    <t>Atualizar o Documento Especificação de Requisitos</t>
+  </si>
+  <si>
+    <t>3.25</t>
   </si>
 </sst>
 </file>
@@ -272,7 +308,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -302,6 +338,10 @@
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -599,20 +639,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I44"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="53.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" customWidth="1"/>
-    <col min="9" max="9" width="56" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="59.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="38.25">
@@ -698,7 +740,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>9</v>
@@ -932,13 +974,13 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" s="16" t="s">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
         <v>9</v>
       </c>
       <c r="C13">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
         <v>12</v>
@@ -947,24 +989,24 @@
         <v>15</v>
       </c>
       <c r="G13" s="6">
-        <v>120</v>
+        <v>82</v>
       </c>
       <c r="H13">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
       </c>
       <c r="C14">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D14" t="s">
         <v>12</v>
@@ -973,10 +1015,10 @@
         <v>15</v>
       </c>
       <c r="G14" s="6">
-        <v>240</v>
-      </c>
-      <c r="H14">
-        <v>210</v>
+        <v>72</v>
+      </c>
+      <c r="H14" s="8">
+        <v>82</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>32</v>
@@ -990,126 +1032,126 @@
         <v>9</v>
       </c>
       <c r="C15">
+        <v>110</v>
+      </c>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="6">
+        <v>62</v>
+      </c>
+      <c r="H15">
+        <v>65</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="D15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F15" t="s">
-        <v>15</v>
-      </c>
-      <c r="G15" s="6">
-        <v>82</v>
-      </c>
-      <c r="H15">
-        <v>90</v>
-      </c>
-      <c r="I15" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="16" t="s">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="6">
+        <v>160</v>
+      </c>
+      <c r="H16" s="8">
+        <v>150</v>
+      </c>
+      <c r="I16" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
+      </c>
+      <c r="D17" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="6">
+        <v>240</v>
+      </c>
+      <c r="H17">
+        <v>210</v>
+      </c>
+      <c r="I17" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>60</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="6">
+        <v>120</v>
+      </c>
+      <c r="H18" s="8">
+        <v>110</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
+      <c r="A19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
-        <v>9</v>
-      </c>
-      <c r="C16">
-        <v>60</v>
-      </c>
-      <c r="D16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="6">
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19">
         <v>110</v>
       </c>
-      <c r="H16">
-        <v>100</v>
-      </c>
-      <c r="I16" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17">
-        <v>40</v>
-      </c>
-      <c r="D17" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="6">
-        <v>72</v>
-      </c>
-      <c r="H17" s="8">
-        <v>82</v>
-      </c>
-      <c r="I17" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18">
-        <v>110</v>
-      </c>
-      <c r="D18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F18" t="s">
-        <v>15</v>
-      </c>
-      <c r="G18" s="6">
+      <c r="D19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="6">
         <v>62</v>
       </c>
-      <c r="H18">
+      <c r="H19">
         <v>65</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I19" s="13" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
-      <c r="A19" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="B19" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19">
-        <v>20</v>
-      </c>
-      <c r="D19" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="6">
-        <v>160</v>
-      </c>
-      <c r="H19" s="8">
-        <v>150</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:9">
@@ -1117,10 +1159,10 @@
         <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C20">
-        <v>60</v>
+        <v>20</v>
       </c>
       <c r="D20" t="s">
         <v>12</v>
@@ -1129,10 +1171,10 @@
         <v>15</v>
       </c>
       <c r="G20" s="6">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="H20" s="8">
-        <v>110</v>
+        <v>150</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>32</v>
@@ -1140,39 +1182,39 @@
     </row>
     <row r="21" spans="1:9">
       <c r="A21" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
       </c>
       <c r="C21">
+        <v>60</v>
+      </c>
+      <c r="D21" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G21" s="6">
         <v>110</v>
       </c>
-      <c r="D21" t="s">
-        <v>12</v>
-      </c>
-      <c r="F21" t="s">
-        <v>15</v>
-      </c>
-      <c r="G21" s="6">
-        <v>62</v>
-      </c>
       <c r="H21">
-        <v>65</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>18</v>
+        <v>100</v>
+      </c>
+      <c r="I21" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="4" t="s">
-        <v>43</v>
+      <c r="A22" t="s">
+        <v>25</v>
       </c>
       <c r="B22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>20</v>
+        <v>80</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -1181,10 +1223,10 @@
         <v>15</v>
       </c>
       <c r="G22" s="6">
-        <v>160</v>
-      </c>
-      <c r="H22" s="8">
-        <v>150</v>
+        <v>120</v>
+      </c>
+      <c r="H22">
+        <v>135</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>32</v>
@@ -1192,7 +1234,7 @@
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -1207,10 +1249,10 @@
         <v>15</v>
       </c>
       <c r="G23" s="6">
-        <v>120</v>
+        <v>240</v>
       </c>
       <c r="H23">
-        <v>135</v>
+        <v>210</v>
       </c>
       <c r="I23" s="11" t="s">
         <v>32</v>
@@ -1218,13 +1260,13 @@
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
       </c>
       <c r="C24">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -1233,10 +1275,10 @@
         <v>15</v>
       </c>
       <c r="G24" s="6">
-        <v>240</v>
+        <v>82</v>
       </c>
       <c r="H24">
-        <v>210</v>
+        <v>90</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>32</v>
@@ -1244,13 +1286,13 @@
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
       <c r="C25">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -1259,10 +1301,10 @@
         <v>15</v>
       </c>
       <c r="G25" s="6">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="H25">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="I25" s="11" t="s">
         <v>32</v>
@@ -1270,13 +1312,13 @@
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
       </c>
       <c r="C26">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1285,10 +1327,10 @@
         <v>15</v>
       </c>
       <c r="G26" s="6">
-        <v>110</v>
+        <v>65</v>
       </c>
       <c r="H26">
-        <v>100</v>
+        <v>35</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>32</v>
@@ -1296,25 +1338,25 @@
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
       </c>
       <c r="C27">
+        <v>80</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="6">
+        <v>82</v>
+      </c>
+      <c r="H27">
         <v>40</v>
-      </c>
-      <c r="D27" t="s">
-        <v>12</v>
-      </c>
-      <c r="F27" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="6">
-        <v>65</v>
-      </c>
-      <c r="H27">
-        <v>35</v>
       </c>
       <c r="I27" s="11" t="s">
         <v>32</v>
@@ -1322,62 +1364,62 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="C28">
-        <v>80</v>
-      </c>
-      <c r="D28" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D28" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
       <c r="G28" s="6">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="H28">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="I28" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" t="s">
-        <v>31</v>
+      <c r="A29" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="B29" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="C29">
-        <v>60</v>
-      </c>
-      <c r="D29" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>12</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
       <c r="G29" s="6">
-        <v>62</v>
+        <v>6</v>
       </c>
       <c r="H29">
-        <v>25</v>
+        <v>4.5</v>
       </c>
       <c r="I29" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:9">
-      <c r="A30" s="14" t="s">
-        <v>49</v>
+      <c r="A30" t="s">
+        <v>48</v>
       </c>
       <c r="B30" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C30">
         <v>100</v>
@@ -1386,20 +1428,254 @@
         <v>12</v>
       </c>
       <c r="F30" t="s">
-        <v>15</v>
-      </c>
-      <c r="G30" s="6">
-        <v>6</v>
-      </c>
-      <c r="H30">
-        <v>4.5</v>
+        <v>49</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="44" spans="6:6">
-      <c r="F44" s="5"/>
+    <row r="31" spans="1:9">
+      <c r="A31" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+      <c r="C31">
+        <v>20</v>
+      </c>
+      <c r="D31" t="s">
+        <v>55</v>
+      </c>
+      <c r="F31" t="s">
+        <v>49</v>
+      </c>
+      <c r="G31" s="6">
+        <v>4</v>
+      </c>
+      <c r="H31" s="18">
+        <v>0</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>60</v>
+      </c>
+      <c r="D32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="6">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="13" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B33" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33" t="s">
+        <v>55</v>
+      </c>
+      <c r="F33" t="s">
+        <v>49</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1</v>
+      </c>
+      <c r="H33" s="17">
+        <v>0</v>
+      </c>
+      <c r="I33" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" t="s">
+        <v>9</v>
+      </c>
+      <c r="C34">
+        <v>40</v>
+      </c>
+      <c r="D34" t="s">
+        <v>55</v>
+      </c>
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="6">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B35" t="s">
+        <v>9</v>
+      </c>
+      <c r="C35">
+        <v>80</v>
+      </c>
+      <c r="D35" t="s">
+        <v>55</v>
+      </c>
+      <c r="F35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" t="s">
+        <v>9</v>
+      </c>
+      <c r="C36">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>55</v>
+      </c>
+      <c r="F36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H36">
+        <v>0</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" t="s">
+        <v>27</v>
+      </c>
+      <c r="B37" t="s">
+        <v>9</v>
+      </c>
+      <c r="C37">
+        <v>40</v>
+      </c>
+      <c r="D37" t="s">
+        <v>55</v>
+      </c>
+      <c r="F37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H37">
+        <v>0</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+      <c r="C38">
+        <v>60</v>
+      </c>
+      <c r="D38" t="s">
+        <v>55</v>
+      </c>
+      <c r="F38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H38">
+        <v>0</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39">
+        <v>60</v>
+      </c>
+      <c r="D39" t="s">
+        <v>55</v>
+      </c>
+      <c r="F39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H39">
+        <v>0</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="F41" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1411,31 +1687,43 @@
     <hyperlink ref="I10" r:id="rId5"/>
     <hyperlink ref="I5" r:id="rId6"/>
     <hyperlink ref="I12" r:id="rId7"/>
-    <hyperlink ref="I17" r:id="rId8"/>
-    <hyperlink ref="I19:I29" r:id="rId9" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I19" r:id="rId10"/>
-    <hyperlink ref="I20" r:id="rId11"/>
-    <hyperlink ref="I23" r:id="rId12"/>
-    <hyperlink ref="I24" r:id="rId13"/>
-    <hyperlink ref="I25" r:id="rId14"/>
-    <hyperlink ref="I26" r:id="rId15"/>
-    <hyperlink ref="I27" r:id="rId16"/>
-    <hyperlink ref="I28" r:id="rId17"/>
-    <hyperlink ref="I29" r:id="rId18"/>
+    <hyperlink ref="I14" r:id="rId8"/>
+    <hyperlink ref="I16:I28" r:id="rId9" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I16" r:id="rId10"/>
+    <hyperlink ref="I18" r:id="rId11"/>
+    <hyperlink ref="I22" r:id="rId12"/>
+    <hyperlink ref="I23" r:id="rId13"/>
+    <hyperlink ref="I24" r:id="rId14"/>
+    <hyperlink ref="I25" r:id="rId15"/>
+    <hyperlink ref="I26" r:id="rId16"/>
+    <hyperlink ref="I27" r:id="rId17"/>
+    <hyperlink ref="I28" r:id="rId18"/>
     <hyperlink ref="I11" r:id="rId19"/>
-    <hyperlink ref="I18" r:id="rId20"/>
-    <hyperlink ref="I22" r:id="rId21"/>
-    <hyperlink ref="I21" r:id="rId22"/>
-    <hyperlink ref="I13:I16" r:id="rId23" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I13" r:id="rId24"/>
-    <hyperlink ref="I14" r:id="rId25"/>
-    <hyperlink ref="I15" r:id="rId26"/>
-    <hyperlink ref="I16" r:id="rId27"/>
-    <hyperlink ref="I4" r:id="rId28"/>
+    <hyperlink ref="I15" r:id="rId20"/>
+    <hyperlink ref="I20" r:id="rId21"/>
+    <hyperlink ref="I19" r:id="rId22"/>
+    <hyperlink ref="I14:I21" r:id="rId23" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I17" r:id="rId24"/>
+    <hyperlink ref="I13" r:id="rId25"/>
+    <hyperlink ref="I21" r:id="rId26"/>
+    <hyperlink ref="I4" r:id="rId27"/>
+    <hyperlink ref="I29" r:id="rId28"/>
     <hyperlink ref="I30" r:id="rId29"/>
+    <hyperlink ref="I31" r:id="rId30"/>
+    <hyperlink ref="I33:I34" r:id="rId31" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I33" r:id="rId32"/>
+    <hyperlink ref="I32" r:id="rId33"/>
+    <hyperlink ref="I31:I34" r:id="rId34" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I34" r:id="rId35"/>
+    <hyperlink ref="I35:I39" r:id="rId36" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I35" r:id="rId37"/>
+    <hyperlink ref="I36" r:id="rId38"/>
+    <hyperlink ref="I37" r:id="rId39"/>
+    <hyperlink ref="I38" r:id="rId40"/>
+    <hyperlink ref="I39" r:id="rId41"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId30"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId42"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atualizar Work Items List
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="62">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1563,8 +1563,8 @@
       <c r="G35" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H35">
-        <v>0</v>
+      <c r="H35" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="I35" s="11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Atualização Plano de Iteração E2
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -641,8 +641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1408,7 +1408,7 @@
         <v>6</v>
       </c>
       <c r="H29">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="I29" s="11" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Criação de novos casos de uso entre outros
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -213,7 +213,7 @@
     <t>8.30</t>
   </si>
   <si>
-    <t>4.10</t>
+    <t>6.10</t>
   </si>
 </sst>
 </file>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>

<commit_message>
Retirar documentos para trabalho fora do ambiente
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -224,7 +224,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -266,6 +266,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF0070C0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -320,7 +326,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -354,6 +360,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -654,7 +664,7 @@
   <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -792,10 +802,10 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="19">
         <v>82</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="20">
         <v>85</v>
       </c>
       <c r="I5" s="13" t="s">

</xml_diff>

<commit_message>
Lista de Trabalho dos documentos fora do ambiente
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="104">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -183,12 +183,6 @@
     <t>Especificar o Caso de Uso Alterar Senha Gerência</t>
   </si>
   <si>
-    <t>Incompleto</t>
-  </si>
-  <si>
-    <t>9.20</t>
-  </si>
-  <si>
     <t>0.20</t>
   </si>
   <si>
@@ -204,16 +198,136 @@
     <t>Correções diversas</t>
   </si>
   <si>
-    <t>Completo</t>
-  </si>
-  <si>
-    <t>Valter</t>
-  </si>
-  <si>
     <t>8.30</t>
   </si>
   <si>
     <t>6.10</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Incluir Cliente</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Incluir Usuário</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Incluir Motorista</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Incluir Veículo</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Incluir Veículo Instalado</t>
+  </si>
+  <si>
+    <t>Criar Tela Incluir Cliente</t>
+  </si>
+  <si>
+    <t>Criar Tela Incluir Usuário</t>
+  </si>
+  <si>
+    <t>Criar Tela Incluir Motorista</t>
+  </si>
+  <si>
+    <t>Criar Tela Incluir Veículo</t>
+  </si>
+  <si>
+    <t>Criar Tela Incluir Veículo Instalado</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Incluir Cliente</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Incluir usuário</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Incluir motorista</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Incluir Veículo</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Incluir Veículo Instalado</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Incluir Cliente</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Incluir Usuário</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Incluir Motorista</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Incluir Veículo</t>
+  </si>
+  <si>
+    <t>Realizar Testes na Tela Incluir Veículo Instalado</t>
+  </si>
+  <si>
+    <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades Tela Alterar Senha Gerencia, Incluir cliente, Incluir Usuário, Incluir Motorista, Incluir Veículo, Incluir veículo Instalado.</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_2</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_3</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_4</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_5</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_6</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_7</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_8</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_9</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_10</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_11</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_12</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_13</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_14</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_15</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_16</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_17</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_18</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_19</t>
+  </si>
+  <si>
+    <t>https://github.com/valtervasconcelos/Projeto_de_Software_20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       1.2</t>
   </si>
 </sst>
 </file>
@@ -271,9 +385,8 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -326,7 +439,7 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -360,10 +473,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -661,10 +783,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I41"/>
+  <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31:D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -777,10 +899,10 @@
         <v>15</v>
       </c>
       <c r="G4" s="6">
-        <v>32</v>
+        <v>48</v>
       </c>
       <c r="H4" s="6">
-        <v>48</v>
+        <v>22</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>18</v>
@@ -802,11 +924,11 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="19">
-        <v>82</v>
-      </c>
-      <c r="H5" s="20">
-        <v>85</v>
+      <c r="G5" s="22">
+        <v>24</v>
+      </c>
+      <c r="H5" s="16">
+        <v>12</v>
       </c>
       <c r="I5" s="13" t="s">
         <v>18</v>
@@ -829,10 +951,10 @@
         <v>15</v>
       </c>
       <c r="G6" s="6">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="H6">
-        <v>145</v>
+        <v>8</v>
       </c>
       <c r="I6" s="13" t="s">
         <v>18</v>
@@ -855,10 +977,10 @@
         <v>15</v>
       </c>
       <c r="G7" s="6">
-        <v>240</v>
+        <v>36</v>
       </c>
       <c r="H7">
-        <v>200</v>
+        <v>30</v>
       </c>
       <c r="I7" s="13" t="s">
         <v>18</v>
@@ -881,10 +1003,10 @@
         <v>15</v>
       </c>
       <c r="G8" s="6">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="H8">
-        <v>70</v>
+        <v>4</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>18</v>
@@ -907,10 +1029,10 @@
         <v>15</v>
       </c>
       <c r="G9" s="6">
-        <v>110</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>90</v>
+        <v>4</v>
       </c>
       <c r="I9" s="13" t="s">
         <v>18</v>
@@ -933,10 +1055,10 @@
         <v>15</v>
       </c>
       <c r="G10" s="6">
-        <v>65</v>
+        <v>4</v>
       </c>
       <c r="H10">
-        <v>70</v>
+        <v>3</v>
       </c>
       <c r="I10" s="13" t="s">
         <v>18</v>
@@ -968,56 +1090,56 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="25.5">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:9">
+      <c r="A12" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>40</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="6">
+        <v>12</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="25.5">
+      <c r="A13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
+      <c r="B13" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13">
         <v>220</v>
       </c>
-      <c r="D12" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F12" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="6">
-        <v>180</v>
-      </c>
-      <c r="H12">
-        <v>160</v>
-      </c>
-      <c r="I12" s="11" t="s">
+      <c r="D13" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="6">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13">
-        <v>40</v>
-      </c>
-      <c r="D13" t="s">
-        <v>12</v>
-      </c>
-      <c r="F13" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="6">
-        <v>82</v>
-      </c>
       <c r="H13">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -1039,8 +1161,8 @@
       <c r="G14" s="6">
         <v>72</v>
       </c>
-      <c r="H14" s="8">
-        <v>82</v>
+      <c r="H14" s="23">
+        <v>36</v>
       </c>
       <c r="I14" s="11" t="s">
         <v>32</v>
@@ -1063,10 +1185,10 @@
         <v>15</v>
       </c>
       <c r="G15" s="6">
-        <v>62</v>
+        <v>36</v>
       </c>
       <c r="H15">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="I15" s="13" t="s">
         <v>18</v>
@@ -1089,10 +1211,10 @@
         <v>15</v>
       </c>
       <c r="G16" s="6">
-        <v>160</v>
+        <v>36</v>
       </c>
       <c r="H16" s="8">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="I16" s="11" t="s">
         <v>32</v>
@@ -1115,10 +1237,10 @@
         <v>15</v>
       </c>
       <c r="G17" s="6">
-        <v>240</v>
+        <v>4</v>
       </c>
       <c r="H17">
-        <v>210</v>
+        <v>3</v>
       </c>
       <c r="I17" s="11" t="s">
         <v>32</v>
@@ -1141,10 +1263,10 @@
         <v>15</v>
       </c>
       <c r="G18" s="6">
-        <v>120</v>
+        <v>24</v>
       </c>
       <c r="H18" s="8">
-        <v>110</v>
+        <v>12</v>
       </c>
       <c r="I18" s="11" t="s">
         <v>32</v>
@@ -1167,10 +1289,10 @@
         <v>15</v>
       </c>
       <c r="G19" s="6">
-        <v>62</v>
+        <v>4</v>
       </c>
       <c r="H19">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="I19" s="13" t="s">
         <v>18</v>
@@ -1193,10 +1315,10 @@
         <v>15</v>
       </c>
       <c r="G20" s="6">
-        <v>160</v>
+        <v>36</v>
       </c>
       <c r="H20" s="8">
-        <v>150</v>
+        <v>36</v>
       </c>
       <c r="I20" s="11" t="s">
         <v>32</v>
@@ -1219,10 +1341,10 @@
         <v>15</v>
       </c>
       <c r="G21" s="6">
-        <v>110</v>
+        <v>6</v>
       </c>
       <c r="H21">
-        <v>100</v>
+        <v>5</v>
       </c>
       <c r="I21" s="11" t="s">
         <v>32</v>
@@ -1236,7 +1358,7 @@
         <v>9</v>
       </c>
       <c r="C22">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="D22" t="s">
         <v>12</v>
@@ -1245,10 +1367,10 @@
         <v>15</v>
       </c>
       <c r="G22" s="6">
-        <v>120</v>
+        <v>2</v>
       </c>
       <c r="H22">
-        <v>135</v>
+        <v>1</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>32</v>
@@ -1262,7 +1384,7 @@
         <v>9</v>
       </c>
       <c r="C23">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
         <v>12</v>
@@ -1271,10 +1393,10 @@
         <v>15</v>
       </c>
       <c r="G23" s="6">
-        <v>240</v>
+        <v>2</v>
       </c>
       <c r="H23">
-        <v>210</v>
+        <v>2</v>
       </c>
       <c r="I23" s="11" t="s">
         <v>32</v>
@@ -1288,7 +1410,7 @@
         <v>9</v>
       </c>
       <c r="C24">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D24" t="s">
         <v>12</v>
@@ -1297,10 +1419,10 @@
         <v>15</v>
       </c>
       <c r="G24" s="6">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="H24">
-        <v>90</v>
+        <v>1</v>
       </c>
       <c r="I24" s="11" t="s">
         <v>32</v>
@@ -1314,7 +1436,7 @@
         <v>9</v>
       </c>
       <c r="C25">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
         <v>12</v>
@@ -1323,10 +1445,10 @@
         <v>15</v>
       </c>
       <c r="G25" s="6">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="I25" s="11" t="s">
         <v>32</v>
@@ -1340,7 +1462,7 @@
         <v>9</v>
       </c>
       <c r="C26">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D26" t="s">
         <v>12</v>
@@ -1349,10 +1471,10 @@
         <v>15</v>
       </c>
       <c r="G26" s="6">
-        <v>65</v>
+        <v>2</v>
       </c>
       <c r="H26">
-        <v>35</v>
+        <v>1</v>
       </c>
       <c r="I26" s="11" t="s">
         <v>32</v>
@@ -1366,7 +1488,7 @@
         <v>9</v>
       </c>
       <c r="C27">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>12</v>
@@ -1375,10 +1497,10 @@
         <v>15</v>
       </c>
       <c r="G27" s="6">
-        <v>82</v>
+        <v>2</v>
       </c>
       <c r="H27">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="I27" s="11" t="s">
         <v>32</v>
@@ -1401,10 +1523,10 @@
         <v>15</v>
       </c>
       <c r="G28" s="6">
-        <v>62</v>
+        <v>1</v>
       </c>
       <c r="H28">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="I28" s="11" t="s">
         <v>32</v>
@@ -1427,10 +1549,10 @@
         <v>15</v>
       </c>
       <c r="G29" s="6">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="H29">
-        <v>5.5</v>
+        <v>42</v>
       </c>
       <c r="I29" s="11" t="s">
         <v>32</v>
@@ -1452,80 +1574,80 @@
       <c r="F30" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="6" t="s">
-        <v>56</v>
+      <c r="G30" s="6">
+        <v>16</v>
       </c>
       <c r="H30" s="6">
-        <v>6.2</v>
+        <v>12</v>
       </c>
       <c r="I30" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:9">
-      <c r="A31" s="4" t="s">
+    <row r="31" spans="1:9" ht="51">
+      <c r="A31" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C31">
+        <v>440</v>
+      </c>
+      <c r="D31" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" t="s">
+        <v>15</v>
+      </c>
+      <c r="G31" s="6">
+        <v>48</v>
+      </c>
+      <c r="H31">
+        <v>36</v>
+      </c>
+      <c r="I31" s="11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
+      <c r="A32" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B31" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31">
-        <v>20</v>
-      </c>
-      <c r="D31" t="s">
-        <v>62</v>
-      </c>
-      <c r="F31" t="s">
-        <v>49</v>
-      </c>
-      <c r="G31" s="6">
+      <c r="B32" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32">
+        <v>120</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" t="s">
+        <v>49</v>
+      </c>
+      <c r="G32" s="6">
         <v>4</v>
       </c>
-      <c r="H31" s="18">
+      <c r="H32" s="18">
         <v>2</v>
       </c>
-      <c r="I31" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="16" t="s">
+      <c r="I32" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B32" t="s">
-        <v>9</v>
-      </c>
-      <c r="C32">
+      <c r="B33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33">
         <v>60</v>
       </c>
-      <c r="D32" t="s">
-        <v>62</v>
-      </c>
-      <c r="F32" t="s">
-        <v>49</v>
-      </c>
-      <c r="G32" s="6">
-        <v>1</v>
-      </c>
-      <c r="H32">
-        <v>1</v>
-      </c>
-      <c r="I32" s="13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B33" t="s">
-        <v>10</v>
-      </c>
-      <c r="C33">
-        <v>10</v>
-      </c>
-      <c r="D33" t="s">
-        <v>62</v>
+      <c r="D33" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="F33" t="s">
         <v>49</v>
@@ -1533,42 +1655,42 @@
       <c r="G33" s="6">
         <v>1</v>
       </c>
-      <c r="H33" s="17">
+      <c r="H33">
         <v>1</v>
       </c>
-      <c r="I33" s="11" t="s">
-        <v>32</v>
+      <c r="I33" s="13" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:9">
-      <c r="A34" s="16" t="s">
+      <c r="A34" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34">
+        <v>10</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" t="s">
+        <v>49</v>
+      </c>
+      <c r="G34" s="6">
+        <v>1</v>
+      </c>
+      <c r="H34" s="17">
+        <v>1</v>
+      </c>
+      <c r="I34" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="16" t="s">
         <v>54</v>
-      </c>
-      <c r="B34" t="s">
-        <v>9</v>
-      </c>
-      <c r="C34">
-        <v>40</v>
-      </c>
-      <c r="D34" t="s">
-        <v>62</v>
-      </c>
-      <c r="F34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G34" s="6">
-        <v>2</v>
-      </c>
-      <c r="H34">
-        <v>1.32</v>
-      </c>
-      <c r="I34" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" t="s">
-        <v>25</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -1576,154 +1698,700 @@
       <c r="C35">
         <v>80</v>
       </c>
-      <c r="D35" t="s">
+      <c r="D35" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
+        <v>49</v>
+      </c>
+      <c r="G35" s="6">
+        <v>4</v>
+      </c>
+      <c r="H35">
+        <v>1.32</v>
+      </c>
+      <c r="I35" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="F35" t="s">
-        <v>49</v>
-      </c>
-      <c r="G35" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="H35">
-        <v>0.15</v>
-      </c>
-      <c r="I35" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9">
-      <c r="A36" t="s">
-        <v>26</v>
-      </c>
-      <c r="B36" t="s">
-        <v>9</v>
+      <c r="B36" s="20" t="s">
+        <v>10</v>
       </c>
       <c r="C36">
         <v>80</v>
       </c>
-      <c r="D36" t="s">
-        <v>62</v>
+      <c r="D36" s="15" t="s">
+        <v>12</v>
       </c>
       <c r="F36" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="6" t="s">
+      <c r="G36" s="6">
+        <v>4</v>
+      </c>
+      <c r="H36">
+        <v>2</v>
+      </c>
+      <c r="I36" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C37">
+        <v>80</v>
+      </c>
+      <c r="D37" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F37" t="s">
+        <v>49</v>
+      </c>
+      <c r="G37" s="6">
+        <v>4</v>
+      </c>
+      <c r="H37">
+        <v>2</v>
+      </c>
+      <c r="I37" s="11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38">
+        <v>80</v>
+      </c>
+      <c r="D38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F38" t="s">
+        <v>49</v>
+      </c>
+      <c r="G38" s="6">
+        <v>4</v>
+      </c>
+      <c r="H38">
+        <v>3</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B39" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C39">
+        <v>80</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F39" t="s">
+        <v>49</v>
+      </c>
+      <c r="G39" s="6">
+        <v>4</v>
+      </c>
+      <c r="H39">
+        <v>2</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="B40" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C40">
+        <v>80</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F40" t="s">
+        <v>49</v>
+      </c>
+      <c r="G40" s="6">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>3</v>
+      </c>
+      <c r="I40" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="19" t="s">
+        <v>67</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41">
+        <v>120</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F41" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="6">
+        <v>36</v>
+      </c>
+      <c r="H41">
+        <v>24</v>
+      </c>
+      <c r="I41" s="11" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B42" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42">
+        <v>120</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F42" t="s">
+        <v>49</v>
+      </c>
+      <c r="G42" s="6">
+        <v>24</v>
+      </c>
+      <c r="H42">
+        <v>12</v>
+      </c>
+      <c r="I42" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C43">
+        <v>120</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F43" t="s">
+        <v>49</v>
+      </c>
+      <c r="G43" s="6">
+        <v>24</v>
+      </c>
+      <c r="H43">
+        <v>8</v>
+      </c>
+      <c r="I43" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="19" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44">
+        <v>120</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F44" t="s">
+        <v>49</v>
+      </c>
+      <c r="G44" s="6">
+        <v>24</v>
+      </c>
+      <c r="H44">
+        <v>8</v>
+      </c>
+      <c r="I44" s="11" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="19" t="s">
+        <v>71</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45">
+        <v>120</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F45" t="s">
+        <v>49</v>
+      </c>
+      <c r="G45" s="6">
+        <v>24</v>
+      </c>
+      <c r="H45">
+        <v>6</v>
+      </c>
+      <c r="I45" s="11" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="21" t="s">
+        <v>72</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46">
+        <v>60</v>
+      </c>
+      <c r="D46" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F46" t="s">
+        <v>49</v>
+      </c>
+      <c r="G46" s="6">
+        <v>2</v>
+      </c>
+      <c r="H46" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I46" s="11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="21" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47">
+        <v>60</v>
+      </c>
+      <c r="D47" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F47" t="s">
+        <v>49</v>
+      </c>
+      <c r="G47" s="6">
+        <v>2</v>
+      </c>
+      <c r="H47" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="I47" s="11" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48">
+        <v>60</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F48" t="s">
+        <v>49</v>
+      </c>
+      <c r="G48" s="6">
+        <v>2</v>
+      </c>
+      <c r="H48" s="16">
+        <v>2</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
+      <c r="A49" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C49">
+        <v>60</v>
+      </c>
+      <c r="D49" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F49" t="s">
+        <v>49</v>
+      </c>
+      <c r="G49" s="6">
+        <v>2</v>
+      </c>
+      <c r="H49" s="16">
+        <v>1</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
+      <c r="A50" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B50" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50">
+        <v>60</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F50" t="s">
+        <v>49</v>
+      </c>
+      <c r="G50" s="6">
+        <v>2</v>
+      </c>
+      <c r="H50" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I50" s="11" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
+      <c r="A51" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B51" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F51" t="s">
+        <v>49</v>
+      </c>
+      <c r="G51" s="6">
+        <v>36</v>
+      </c>
+      <c r="H51">
+        <v>36</v>
+      </c>
+      <c r="I51" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
+      <c r="A52" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C52">
+        <v>10</v>
+      </c>
+      <c r="D52" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F52" t="s">
+        <v>49</v>
+      </c>
+      <c r="G52" s="6">
+        <v>36</v>
+      </c>
+      <c r="H52">
+        <v>36</v>
+      </c>
+      <c r="I52" s="11" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
+      <c r="A53" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C53">
+        <v>10</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F53" t="s">
+        <v>49</v>
+      </c>
+      <c r="G53" s="6">
+        <v>36</v>
+      </c>
+      <c r="H53">
+        <v>36</v>
+      </c>
+      <c r="I53" s="11" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
+      <c r="A54" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C54">
+        <v>10</v>
+      </c>
+      <c r="D54" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F54" t="s">
+        <v>49</v>
+      </c>
+      <c r="G54" s="6">
+        <v>36</v>
+      </c>
+      <c r="H54">
+        <v>36</v>
+      </c>
+      <c r="I54" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9">
+      <c r="A55" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B55" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F55" t="s">
+        <v>49</v>
+      </c>
+      <c r="G55" s="6">
+        <v>36</v>
+      </c>
+      <c r="H55">
+        <v>36</v>
+      </c>
+      <c r="I55" s="11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9">
+      <c r="A56" t="s">
+        <v>25</v>
+      </c>
+      <c r="B56" t="s">
+        <v>9</v>
+      </c>
+      <c r="C56">
+        <v>30</v>
+      </c>
+      <c r="D56" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F56" t="s">
+        <v>49</v>
+      </c>
+      <c r="G56" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H56">
+        <v>0.15</v>
+      </c>
+      <c r="I56" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9">
+      <c r="A57" t="s">
+        <v>26</v>
+      </c>
+      <c r="B57" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57">
+        <v>30</v>
+      </c>
+      <c r="D57" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F57" t="s">
+        <v>49</v>
+      </c>
+      <c r="G57" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H57">
+        <v>0.15</v>
+      </c>
+      <c r="I57" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" t="s">
+        <v>27</v>
+      </c>
+      <c r="B58" t="s">
+        <v>9</v>
+      </c>
+      <c r="C58">
+        <v>30</v>
+      </c>
+      <c r="D58" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F58" t="s">
+        <v>49</v>
+      </c>
+      <c r="G58" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H58">
+        <v>0.15</v>
+      </c>
+      <c r="I58" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" t="s">
+        <v>28</v>
+      </c>
+      <c r="B59" t="s">
+        <v>9</v>
+      </c>
+      <c r="C59">
+        <v>30</v>
+      </c>
+      <c r="D59" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F59" t="s">
+        <v>49</v>
+      </c>
+      <c r="G59" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H36">
+      <c r="H59">
         <v>0.15</v>
       </c>
-      <c r="I36" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" t="s">
-        <v>27</v>
-      </c>
-      <c r="B37" t="s">
-        <v>9</v>
-      </c>
-      <c r="C37">
-        <v>40</v>
-      </c>
-      <c r="D37" t="s">
-        <v>62</v>
-      </c>
-      <c r="F37" t="s">
-        <v>49</v>
-      </c>
-      <c r="G37" s="6" t="s">
+      <c r="I59" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" t="s">
         <v>58</v>
       </c>
-      <c r="H37">
+      <c r="B60" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60">
+        <v>30</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F60" t="s">
+        <v>49</v>
+      </c>
+      <c r="G60" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H60">
         <v>0.15</v>
       </c>
-      <c r="I37" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9">
-      <c r="A38" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" t="s">
-        <v>9</v>
-      </c>
-      <c r="C38">
+      <c r="I60" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" t="s">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>9</v>
+      </c>
+      <c r="C61">
+        <v>20</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F61" t="s">
+        <v>49</v>
+      </c>
+      <c r="G61" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="D38" t="s">
-        <v>62</v>
-      </c>
-      <c r="F38" t="s">
-        <v>49</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H38">
-        <v>0.15</v>
-      </c>
-      <c r="I38" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" t="s">
-        <v>60</v>
-      </c>
-      <c r="B39" t="s">
-        <v>34</v>
-      </c>
-      <c r="C39">
-        <v>60</v>
-      </c>
-      <c r="D39" t="s">
-        <v>62</v>
-      </c>
-      <c r="F39" t="s">
-        <v>49</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="H39">
-        <v>0.15</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9">
-      <c r="A40" t="s">
+      <c r="H61" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B40" t="s">
-        <v>9</v>
-      </c>
-      <c r="C40">
-        <v>20</v>
-      </c>
-      <c r="D40" t="s">
-        <v>55</v>
-      </c>
-      <c r="F40" t="s">
-        <v>63</v>
-      </c>
-      <c r="G40" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="H40" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9">
-      <c r="F41" s="5"/>
+      <c r="I61" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="F62" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -1734,7 +2402,7 @@
     <hyperlink ref="I9" r:id="rId4"/>
     <hyperlink ref="I10" r:id="rId5"/>
     <hyperlink ref="I5" r:id="rId6"/>
-    <hyperlink ref="I12" r:id="rId7"/>
+    <hyperlink ref="I13" r:id="rId7"/>
     <hyperlink ref="I14" r:id="rId8"/>
     <hyperlink ref="I16:I28" r:id="rId9" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
     <hyperlink ref="I16" r:id="rId10"/>
@@ -1752,27 +2420,30 @@
     <hyperlink ref="I19" r:id="rId22"/>
     <hyperlink ref="I14:I21" r:id="rId23" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
     <hyperlink ref="I17" r:id="rId24"/>
-    <hyperlink ref="I13" r:id="rId25"/>
+    <hyperlink ref="I12" r:id="rId25"/>
     <hyperlink ref="I21" r:id="rId26"/>
     <hyperlink ref="I4" r:id="rId27"/>
     <hyperlink ref="I29" r:id="rId28"/>
     <hyperlink ref="I30" r:id="rId29"/>
-    <hyperlink ref="I31" r:id="rId30"/>
-    <hyperlink ref="I33:I34" r:id="rId31" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I33" r:id="rId32"/>
-    <hyperlink ref="I32" r:id="rId33"/>
-    <hyperlink ref="I31:I34" r:id="rId34" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I34" r:id="rId35"/>
-    <hyperlink ref="I35:I39" r:id="rId36" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I35" r:id="rId37"/>
-    <hyperlink ref="I36" r:id="rId38"/>
-    <hyperlink ref="I37" r:id="rId39"/>
-    <hyperlink ref="I38" r:id="rId40"/>
-    <hyperlink ref="I39" r:id="rId41"/>
-    <hyperlink ref="I40" r:id="rId42"/>
+    <hyperlink ref="I32" r:id="rId30"/>
+    <hyperlink ref="I34:I35" r:id="rId31" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I34" r:id="rId32"/>
+    <hyperlink ref="I33" r:id="rId33"/>
+    <hyperlink ref="I32:I35" r:id="rId34" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I35" r:id="rId35"/>
+    <hyperlink ref="I56:I60" r:id="rId36" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I56" r:id="rId37"/>
+    <hyperlink ref="I57" r:id="rId38"/>
+    <hyperlink ref="I58" r:id="rId39"/>
+    <hyperlink ref="I59" r:id="rId40"/>
+    <hyperlink ref="I60" r:id="rId41"/>
+    <hyperlink ref="I61" r:id="rId42"/>
+    <hyperlink ref="I31" r:id="rId43"/>
+    <hyperlink ref="I36" r:id="rId44"/>
+    <hyperlink ref="I37:I55" r:id="rId45" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId43"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId46"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atualizar Work_list_Sistema de Rastreamento
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="103">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -324,10 +324,7 @@
     <t>https://github.com/valtervasconcelos/Projeto_de_Software_20</t>
   </si>
   <si>
-    <t xml:space="preserve">                       1.3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                       1.2</t>
+    <t>Incompleto</t>
   </si>
 </sst>
 </file>
@@ -785,8 +782,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31:D61"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1985,7 +1982,7 @@
         <v>60</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F46" t="s">
         <v>49</v>
@@ -1993,8 +1990,8 @@
       <c r="G46" s="6">
         <v>2</v>
       </c>
-      <c r="H46" s="16" t="s">
-        <v>102</v>
+      <c r="H46" s="16">
+        <v>0</v>
       </c>
       <c r="I46" s="11" t="s">
         <v>92</v>
@@ -2011,7 +2008,7 @@
         <v>60</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F47" t="s">
         <v>49</v>
@@ -2019,8 +2016,8 @@
       <c r="G47" s="6">
         <v>2</v>
       </c>
-      <c r="H47" s="16" t="s">
-        <v>103</v>
+      <c r="H47" s="16">
+        <v>0</v>
       </c>
       <c r="I47" s="11" t="s">
         <v>93</v>
@@ -2037,7 +2034,7 @@
         <v>60</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F48" t="s">
         <v>49</v>
@@ -2046,7 +2043,7 @@
         <v>2</v>
       </c>
       <c r="H48" s="16">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I48" s="11" t="s">
         <v>94</v>
@@ -2063,7 +2060,7 @@
         <v>60</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F49" t="s">
         <v>49</v>
@@ -2072,7 +2069,7 @@
         <v>2</v>
       </c>
       <c r="H49" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I49" s="11" t="s">
         <v>95</v>
@@ -2089,7 +2086,7 @@
         <v>60</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F50" t="s">
         <v>49</v>
@@ -2097,8 +2094,8 @@
       <c r="G50" s="6">
         <v>2</v>
       </c>
-      <c r="H50" s="16" t="s">
-        <v>102</v>
+      <c r="H50" s="16">
+        <v>0</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>96</v>
@@ -2115,7 +2112,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F51" t="s">
         <v>49</v>
@@ -2124,7 +2121,7 @@
         <v>36</v>
       </c>
       <c r="H51">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I51" s="11" t="s">
         <v>97</v>
@@ -2141,7 +2138,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F52" t="s">
         <v>49</v>
@@ -2150,7 +2147,7 @@
         <v>36</v>
       </c>
       <c r="H52">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I52" s="11" t="s">
         <v>98</v>
@@ -2167,7 +2164,7 @@
         <v>10</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F53" t="s">
         <v>49</v>
@@ -2176,7 +2173,7 @@
         <v>36</v>
       </c>
       <c r="H53">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I53" s="11" t="s">
         <v>99</v>
@@ -2193,7 +2190,7 @@
         <v>10</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F54" t="s">
         <v>49</v>
@@ -2202,7 +2199,7 @@
         <v>36</v>
       </c>
       <c r="H54">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I54" s="11" t="s">
         <v>100</v>
@@ -2219,7 +2216,7 @@
         <v>10</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>12</v>
+        <v>102</v>
       </c>
       <c r="F55" t="s">
         <v>49</v>
@@ -2228,7 +2225,7 @@
         <v>36</v>
       </c>
       <c r="H55">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="I55" s="11" t="s">
         <v>101</v>

</xml_diff>

<commit_message>
Atualizar lista de trabalho
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="107">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -331,6 +331,12 @@
   </si>
   <si>
     <t>2.5</t>
+  </si>
+  <si>
+    <t>Organizar documentos UML`s em pacotes</t>
+  </si>
+  <si>
+    <t>Valter</t>
   </si>
 </sst>
 </file>
@@ -788,8 +794,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="90" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2394,7 +2400,30 @@
       </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="F62" s="5"/>
+      <c r="A62" t="s">
+        <v>105</v>
+      </c>
+      <c r="B62" t="s">
+        <v>10</v>
+      </c>
+      <c r="C62">
+        <v>40</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F62" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="G62">
+        <v>4</v>
+      </c>
+      <c r="H62">
+        <v>2</v>
+      </c>
+      <c r="I62" s="11" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2444,9 +2473,10 @@
     <hyperlink ref="I31" r:id="rId43"/>
     <hyperlink ref="I36" r:id="rId44"/>
     <hyperlink ref="I37:I55" r:id="rId45" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I62" r:id="rId46"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId46"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId47"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atualização de Lista de trabalho
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="90">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -264,63 +264,6 @@
     <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades Tela Alterar Senha Gerencia, Incluir cliente, Incluir Usuário, Incluir Motorista, Incluir Veículo, Incluir veículo Instalado.</t>
   </si>
   <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_2</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_3</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_4</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_5</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_6</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_7</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_8</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_9</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_10</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_11</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_12</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_13</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_14</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_15</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_16</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_17</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_18</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_19</t>
-  </si>
-  <si>
-    <t>https://github.com/valtervasconcelos/Projeto_de_Software_20</t>
-  </si>
-  <si>
     <t>Incompleto</t>
   </si>
   <si>
@@ -337,6 +280,12 @@
   </si>
   <si>
     <t>Valter</t>
+  </si>
+  <si>
+    <t>Atualizar documento Script de teste</t>
+  </si>
+  <si>
+    <t>incompleto</t>
   </si>
 </sst>
 </file>
@@ -792,10 +741,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B37" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I62" sqref="I62"/>
+    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34:I55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1772,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="I37" s="11" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:9">
@@ -1798,7 +1747,7 @@
         <v>3</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>83</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9">
@@ -1824,7 +1773,7 @@
         <v>2</v>
       </c>
       <c r="I39" s="11" t="s">
-        <v>84</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:9">
@@ -1850,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>85</v>
+        <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:9">
@@ -1876,7 +1825,7 @@
         <v>24</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>86</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:9">
@@ -1902,7 +1851,7 @@
         <v>12</v>
       </c>
       <c r="I42" s="11" t="s">
-        <v>87</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:9">
@@ -1928,7 +1877,7 @@
         <v>8</v>
       </c>
       <c r="I43" s="11" t="s">
-        <v>88</v>
+        <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:9">
@@ -1954,7 +1903,7 @@
         <v>8</v>
       </c>
       <c r="I44" s="11" t="s">
-        <v>89</v>
+        <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:9">
@@ -1980,7 +1929,7 @@
         <v>6</v>
       </c>
       <c r="I45" s="11" t="s">
-        <v>90</v>
+        <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:9">
@@ -1994,19 +1943,19 @@
         <v>60</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F46" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="I46" s="11" t="s">
-        <v>91</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -2020,19 +1969,19 @@
         <v>60</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F47" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H47" s="16">
         <v>2</v>
       </c>
       <c r="I47" s="11" t="s">
-        <v>92</v>
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -2046,19 +1995,19 @@
         <v>60</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F48" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H48" s="22">
         <v>2.5</v>
       </c>
       <c r="I48" s="11" t="s">
-        <v>93</v>
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -2072,19 +2021,19 @@
         <v>60</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F49" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H49" s="22">
         <v>1.7</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>94</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:9">
@@ -2098,19 +2047,19 @@
         <v>60</v>
       </c>
       <c r="D50" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F50" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="H50" s="16">
         <v>3</v>
       </c>
       <c r="I50" s="11" t="s">
-        <v>95</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:9">
@@ -2124,10 +2073,10 @@
         <v>10</v>
       </c>
       <c r="D51" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F51" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G51" s="6">
         <v>36</v>
@@ -2136,7 +2085,7 @@
         <v>32</v>
       </c>
       <c r="I51" s="11" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:9">
@@ -2150,10 +2099,10 @@
         <v>10</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F52" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G52" s="6">
         <v>36</v>
@@ -2162,7 +2111,7 @@
         <v>18</v>
       </c>
       <c r="I52" s="11" t="s">
-        <v>97</v>
+        <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:9">
@@ -2176,10 +2125,10 @@
         <v>10</v>
       </c>
       <c r="D53" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F53" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G53" s="6">
         <v>36</v>
@@ -2188,7 +2137,7 @@
         <v>22</v>
       </c>
       <c r="I53" s="11" t="s">
-        <v>98</v>
+        <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:9">
@@ -2202,10 +2151,10 @@
         <v>10</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F54" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G54" s="6">
         <v>36</v>
@@ -2214,7 +2163,7 @@
         <v>25</v>
       </c>
       <c r="I54" s="11" t="s">
-        <v>99</v>
+        <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2228,10 +2177,10 @@
         <v>10</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="F55" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G55" s="6">
         <v>36</v>
@@ -2240,7 +2189,7 @@
         <v>25</v>
       </c>
       <c r="I55" s="11" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2401,7 +2350,7 @@
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -2410,10 +2359,10 @@
         <v>40</v>
       </c>
       <c r="D62" s="15" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="G62">
         <v>4</v>
@@ -2422,6 +2371,32 @@
         <v>2</v>
       </c>
       <c r="I62" s="11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" t="s">
+        <v>88</v>
+      </c>
+      <c r="B63" t="s">
+        <v>10</v>
+      </c>
+      <c r="C63">
+        <v>70</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="F63" t="s">
+        <v>83</v>
+      </c>
+      <c r="G63">
+        <v>4</v>
+      </c>
+      <c r="H63">
+        <v>3</v>
+      </c>
+      <c r="I63" s="11" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2462,21 +2437,20 @@
     <hyperlink ref="I34" r:id="rId32"/>
     <hyperlink ref="I33" r:id="rId33"/>
     <hyperlink ref="I32:I35" r:id="rId34" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I35" r:id="rId35"/>
-    <hyperlink ref="I56:I60" r:id="rId36" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I56" r:id="rId37"/>
-    <hyperlink ref="I57" r:id="rId38"/>
-    <hyperlink ref="I58" r:id="rId39"/>
-    <hyperlink ref="I59" r:id="rId40"/>
-    <hyperlink ref="I60" r:id="rId41"/>
-    <hyperlink ref="I61" r:id="rId42"/>
-    <hyperlink ref="I31" r:id="rId43"/>
-    <hyperlink ref="I36" r:id="rId44"/>
-    <hyperlink ref="I37:I55" r:id="rId45" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
-    <hyperlink ref="I62" r:id="rId46"/>
+    <hyperlink ref="I56:I60" r:id="rId35" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I56" r:id="rId36"/>
+    <hyperlink ref="I57" r:id="rId37"/>
+    <hyperlink ref="I58" r:id="rId38"/>
+    <hyperlink ref="I59" r:id="rId39"/>
+    <hyperlink ref="I60" r:id="rId40"/>
+    <hyperlink ref="I61" r:id="rId41"/>
+    <hyperlink ref="I31" r:id="rId42"/>
+    <hyperlink ref="I62" r:id="rId43"/>
+    <hyperlink ref="I63" r:id="rId44"/>
+    <hyperlink ref="I35:I55" r:id="rId45" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId47"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId46"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atualizar Planilha de Ítens de Trabalho
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="90">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -296,7 +296,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -308,12 +308,6 @@
     </font>
     <font>
       <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -393,11 +387,11 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -407,7 +401,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -415,11 +408,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -434,7 +427,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -743,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I34" sqref="I34:I55"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H62" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -804,13 +797,13 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="I2" s="11" t="s">
         <v>13</v>
       </c>
     </row>
@@ -830,39 +823,39 @@
       <c r="F3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="11" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="B4" s="15" t="s">
         <v>9</v>
       </c>
       <c r="C4">
         <v>50</v>
       </c>
-      <c r="D4" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="6">
+      <c r="D4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="5">
         <v>48</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>22</v>
       </c>
-      <c r="I4" s="13" t="s">
+      <c r="I4" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -882,13 +875,13 @@
       <c r="F5" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>24</v>
       </c>
-      <c r="H5" s="16">
-        <v>12</v>
-      </c>
-      <c r="I5" s="13" t="s">
+      <c r="H5" s="15">
+        <v>12</v>
+      </c>
+      <c r="I5" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -908,13 +901,13 @@
       <c r="F6" t="s">
         <v>15</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="5">
         <v>24</v>
       </c>
       <c r="H6">
         <v>8</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -934,13 +927,13 @@
       <c r="F7" t="s">
         <v>15</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="5">
         <v>36</v>
       </c>
       <c r="H7">
         <v>30</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -960,13 +953,13 @@
       <c r="F8" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="5">
         <v>6</v>
       </c>
       <c r="H8">
         <v>4</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -986,13 +979,13 @@
       <c r="F9" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="5">
         <v>8</v>
       </c>
       <c r="H9">
         <v>4</v>
       </c>
-      <c r="I9" s="13" t="s">
+      <c r="I9" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1012,13 +1005,13 @@
       <c r="F10" t="s">
         <v>15</v>
       </c>
-      <c r="G10" s="6">
+      <c r="G10" s="5">
         <v>4</v>
       </c>
       <c r="H10">
         <v>3</v>
       </c>
-      <c r="I10" s="13" t="s">
+      <c r="I10" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1038,18 +1031,18 @@
       <c r="F11" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="5">
         <v>2</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="15" t="s">
         <v>50</v>
       </c>
       <c r="B12" t="s">
@@ -1064,39 +1057,39 @@
       <c r="F12" t="s">
         <v>15</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="5">
         <v>12</v>
       </c>
       <c r="H12">
         <v>8</v>
       </c>
-      <c r="I12" s="11" t="s">
+      <c r="I12" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="25.5">
-      <c r="A13" s="14" t="s">
+      <c r="A13" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C13">
         <v>220</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F13" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="5">
         <v>24</v>
       </c>
       <c r="H13">
         <v>24</v>
       </c>
-      <c r="I13" s="11" t="s">
+      <c r="I13" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1116,18 +1109,18 @@
       <c r="F14" t="s">
         <v>15</v>
       </c>
-      <c r="G14" s="6">
+      <c r="G14" s="5">
         <v>72</v>
       </c>
-      <c r="H14" s="23">
+      <c r="H14" s="22">
         <v>36</v>
       </c>
-      <c r="I14" s="11" t="s">
+      <c r="I14" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="16" t="s">
+      <c r="A15" s="15" t="s">
         <v>45</v>
       </c>
       <c r="B15" t="s">
@@ -1142,13 +1135,13 @@
       <c r="F15" t="s">
         <v>15</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="5">
         <v>36</v>
       </c>
       <c r="H15">
         <v>36</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="I15" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1168,18 +1161,18 @@
       <c r="F16" t="s">
         <v>15</v>
       </c>
-      <c r="G16" s="6">
+      <c r="G16" s="5">
         <v>36</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="7">
         <v>36</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="15" t="s">
         <v>38</v>
       </c>
       <c r="B17" t="s">
@@ -1194,13 +1187,13 @@
       <c r="F17" t="s">
         <v>15</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="5">
         <v>4</v>
       </c>
       <c r="H17">
         <v>3</v>
       </c>
-      <c r="I17" s="11" t="s">
+      <c r="I17" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1220,18 +1213,18 @@
       <c r="F18" t="s">
         <v>15</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="5">
         <v>24</v>
       </c>
-      <c r="H18" s="8">
-        <v>12</v>
-      </c>
-      <c r="I18" s="11" t="s">
+      <c r="H18" s="7">
+        <v>12</v>
+      </c>
+      <c r="I18" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="16" t="s">
+      <c r="A19" s="15" t="s">
         <v>46</v>
       </c>
       <c r="B19" t="s">
@@ -1246,13 +1239,13 @@
       <c r="F19" t="s">
         <v>15</v>
       </c>
-      <c r="G19" s="6">
+      <c r="G19" s="5">
         <v>4</v>
       </c>
       <c r="H19">
         <v>2</v>
       </c>
-      <c r="I19" s="13" t="s">
+      <c r="I19" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1272,18 +1265,18 @@
       <c r="F20" t="s">
         <v>15</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="5">
         <v>36</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="7">
         <v>36</v>
       </c>
-      <c r="I20" s="11" t="s">
+      <c r="I20" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="16" t="s">
+      <c r="A21" s="15" t="s">
         <v>44</v>
       </c>
       <c r="B21" t="s">
@@ -1298,13 +1291,13 @@
       <c r="F21" t="s">
         <v>15</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="5">
         <v>6</v>
       </c>
       <c r="H21">
         <v>5</v>
       </c>
-      <c r="I21" s="11" t="s">
+      <c r="I21" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1324,13 +1317,13 @@
       <c r="F22" t="s">
         <v>15</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="5">
         <v>2</v>
       </c>
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" s="11" t="s">
+      <c r="I22" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1350,13 +1343,13 @@
       <c r="F23" t="s">
         <v>15</v>
       </c>
-      <c r="G23" s="6">
+      <c r="G23" s="5">
         <v>2</v>
       </c>
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23" s="11" t="s">
+      <c r="I23" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1376,13 +1369,13 @@
       <c r="F24" t="s">
         <v>15</v>
       </c>
-      <c r="G24" s="6">
+      <c r="G24" s="5">
         <v>2</v>
       </c>
       <c r="H24">
         <v>1</v>
       </c>
-      <c r="I24" s="11" t="s">
+      <c r="I24" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1402,13 +1395,13 @@
       <c r="F25" t="s">
         <v>15</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="5">
         <v>1</v>
       </c>
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25" s="11" t="s">
+      <c r="I25" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1428,13 +1421,13 @@
       <c r="F26" t="s">
         <v>15</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="5">
         <v>2</v>
       </c>
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26" s="11" t="s">
+      <c r="I26" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1448,19 +1441,19 @@
       <c r="C27">
         <v>30</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="9" t="s">
         <v>12</v>
       </c>
       <c r="F27" t="s">
         <v>15</v>
       </c>
-      <c r="G27" s="6">
+      <c r="G27" s="5">
         <v>2</v>
       </c>
       <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27" s="11" t="s">
+      <c r="I27" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1474,24 +1467,24 @@
       <c r="C28">
         <v>60</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D28" s="8" t="s">
         <v>12</v>
       </c>
       <c r="F28" t="s">
         <v>15</v>
       </c>
-      <c r="G28" s="6">
+      <c r="G28" s="5">
         <v>1</v>
       </c>
       <c r="H28">
         <v>1</v>
       </c>
-      <c r="I28" s="11" t="s">
+      <c r="I28" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="14" t="s">
+      <c r="A29" s="13" t="s">
         <v>47</v>
       </c>
       <c r="B29" t="s">
@@ -1500,19 +1493,19 @@
       <c r="C29">
         <v>100</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F29" t="s">
         <v>15</v>
       </c>
-      <c r="G29" s="6">
+      <c r="G29" s="5">
         <v>48</v>
       </c>
       <c r="H29">
         <v>42</v>
       </c>
-      <c r="I29" s="11" t="s">
+      <c r="I29" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1526,45 +1519,45 @@
       <c r="C30">
         <v>100</v>
       </c>
-      <c r="D30" s="7" t="s">
+      <c r="D30" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F30" t="s">
         <v>49</v>
       </c>
-      <c r="G30" s="6">
+      <c r="G30" s="5">
         <v>16</v>
       </c>
-      <c r="H30" s="6">
-        <v>12</v>
-      </c>
-      <c r="I30" s="11" t="s">
+      <c r="H30" s="5">
+        <v>12</v>
+      </c>
+      <c r="I30" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:9" ht="51">
-      <c r="A31" s="14" t="s">
+      <c r="A31" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="B31" s="16" t="s">
+      <c r="B31" s="15" t="s">
         <v>10</v>
       </c>
       <c r="C31">
         <v>440</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F31" t="s">
         <v>15</v>
       </c>
-      <c r="G31" s="6">
+      <c r="G31" s="5">
         <v>48</v>
       </c>
       <c r="H31">
         <v>36</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="10" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1578,24 +1571,24 @@
       <c r="C32">
         <v>120</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F32" t="s">
         <v>49</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="5">
         <v>4</v>
       </c>
-      <c r="H32" s="18">
+      <c r="H32" s="17">
         <v>2</v>
       </c>
-      <c r="I32" s="11" t="s">
+      <c r="I32" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="15" t="s">
         <v>52</v>
       </c>
       <c r="B33" t="s">
@@ -1604,19 +1597,19 @@
       <c r="C33">
         <v>60</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F33" t="s">
         <v>49</v>
       </c>
-      <c r="G33" s="6">
+      <c r="G33" s="5">
         <v>1</v>
       </c>
       <c r="H33">
         <v>1</v>
       </c>
-      <c r="I33" s="13" t="s">
+      <c r="I33" s="12" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1630,24 +1623,24 @@
       <c r="C34">
         <v>10</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F34" t="s">
         <v>49</v>
       </c>
-      <c r="G34" s="6">
+      <c r="G34" s="5">
         <v>1</v>
       </c>
-      <c r="H34" s="17">
+      <c r="H34" s="16">
         <v>1</v>
       </c>
-      <c r="I34" s="11" t="s">
+      <c r="I34" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="15" t="s">
         <v>54</v>
       </c>
       <c r="B35" t="s">
@@ -1656,539 +1649,539 @@
       <c r="C35">
         <v>80</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F35" t="s">
         <v>49</v>
       </c>
-      <c r="G35" s="6">
+      <c r="G35" s="5">
         <v>4</v>
       </c>
       <c r="H35">
         <v>1.32</v>
       </c>
-      <c r="I35" s="11" t="s">
+      <c r="I35" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="19" t="s">
+      <c r="A36" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C36">
         <v>80</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F36" t="s">
         <v>49</v>
       </c>
-      <c r="G36" s="6">
+      <c r="G36" s="5">
         <v>4</v>
       </c>
       <c r="H36">
         <v>2</v>
       </c>
-      <c r="I36" s="11" t="s">
+      <c r="I36" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="19" t="s">
+      <c r="A37" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C37">
         <v>80</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F37" t="s">
         <v>49</v>
       </c>
-      <c r="G37" s="6">
+      <c r="G37" s="5">
         <v>4</v>
       </c>
       <c r="H37">
         <v>2</v>
       </c>
-      <c r="I37" s="11" t="s">
+      <c r="I37" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="19" t="s">
+      <c r="A38" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C38">
         <v>80</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F38" t="s">
         <v>49</v>
       </c>
-      <c r="G38" s="6">
+      <c r="G38" s="5">
         <v>4</v>
       </c>
       <c r="H38">
         <v>3</v>
       </c>
-      <c r="I38" s="11" t="s">
+      <c r="I38" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="19" t="s">
+      <c r="A39" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C39">
         <v>80</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F39" t="s">
         <v>49</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="5">
         <v>4</v>
       </c>
       <c r="H39">
         <v>2</v>
       </c>
-      <c r="I39" s="11" t="s">
+      <c r="I39" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="19" t="s">
+      <c r="A40" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B40" s="20" t="s">
+      <c r="B40" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C40">
         <v>80</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F40" t="s">
         <v>49</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="5">
         <v>4</v>
       </c>
       <c r="H40">
         <v>3</v>
       </c>
-      <c r="I40" s="11" t="s">
+      <c r="I40" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="19" t="s">
+      <c r="A41" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B41" s="20" t="s">
+      <c r="B41" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C41">
         <v>120</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F41" t="s">
         <v>49</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="5">
         <v>36</v>
       </c>
       <c r="H41">
         <v>24</v>
       </c>
-      <c r="I41" s="11" t="s">
+      <c r="I41" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C42">
         <v>120</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F42" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="6">
+      <c r="G42" s="5">
         <v>24</v>
       </c>
       <c r="H42">
         <v>12</v>
       </c>
-      <c r="I42" s="11" t="s">
+      <c r="I42" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C43">
         <v>120</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F43" t="s">
         <v>49</v>
       </c>
-      <c r="G43" s="6">
+      <c r="G43" s="5">
         <v>24</v>
       </c>
       <c r="H43">
         <v>8</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="I43" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C44">
         <v>120</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F44" t="s">
         <v>49</v>
       </c>
-      <c r="G44" s="6">
+      <c r="G44" s="5">
         <v>24</v>
       </c>
       <c r="H44">
         <v>8</v>
       </c>
-      <c r="I44" s="11" t="s">
+      <c r="I44" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B45" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C45">
         <v>120</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F45" t="s">
         <v>49</v>
       </c>
-      <c r="G45" s="6">
+      <c r="G45" s="5">
         <v>24</v>
       </c>
       <c r="H45">
         <v>6</v>
       </c>
-      <c r="I45" s="11" t="s">
+      <c r="I45" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="21" t="s">
+      <c r="A46" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C46">
         <v>60</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F46" t="s">
         <v>83</v>
       </c>
-      <c r="G46" s="6" t="s">
+      <c r="G46" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="I46" s="11" t="s">
+      <c r="I46" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="21" t="s">
+      <c r="A47" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C47">
         <v>60</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F47" t="s">
         <v>83</v>
       </c>
-      <c r="G47" s="6" t="s">
+      <c r="G47" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H47" s="16">
+      <c r="H47" s="15">
         <v>2</v>
       </c>
-      <c r="I47" s="11" t="s">
+      <c r="I47" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="21" t="s">
+      <c r="A48" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C48">
         <v>60</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F48" t="s">
         <v>83</v>
       </c>
-      <c r="G48" s="6" t="s">
+      <c r="G48" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H48" s="22">
+      <c r="H48" s="21">
         <v>2.5</v>
       </c>
-      <c r="I48" s="11" t="s">
+      <c r="I48" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="21" t="s">
+      <c r="A49" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C49">
         <v>60</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F49" t="s">
         <v>83</v>
       </c>
-      <c r="G49" s="6" t="s">
+      <c r="G49" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H49" s="22">
+      <c r="H49" s="21">
         <v>1.7</v>
       </c>
-      <c r="I49" s="11" t="s">
+      <c r="I49" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C50">
         <v>60</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F50" t="s">
         <v>83</v>
       </c>
-      <c r="G50" s="6" t="s">
+      <c r="G50" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="H50" s="16">
+      <c r="H50" s="15">
         <v>3</v>
       </c>
-      <c r="I50" s="11" t="s">
+      <c r="I50" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="21" t="s">
+      <c r="A51" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C51">
         <v>10</v>
       </c>
-      <c r="D51" s="15" t="s">
+      <c r="D51" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F51" t="s">
         <v>83</v>
       </c>
-      <c r="G51" s="6">
+      <c r="G51" s="5">
         <v>36</v>
       </c>
       <c r="H51">
         <v>32</v>
       </c>
-      <c r="I51" s="11" t="s">
+      <c r="I51" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="20" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C52">
         <v>10</v>
       </c>
-      <c r="D52" s="15" t="s">
+      <c r="D52" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F52" t="s">
         <v>83</v>
       </c>
-      <c r="G52" s="6">
+      <c r="G52" s="5">
         <v>36</v>
       </c>
       <c r="H52">
         <v>18</v>
       </c>
-      <c r="I52" s="11" t="s">
+      <c r="I52" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="21" t="s">
+      <c r="A53" s="20" t="s">
         <v>78</v>
       </c>
-      <c r="B53" s="20" t="s">
+      <c r="B53" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C53">
         <v>10</v>
       </c>
-      <c r="D53" s="15" t="s">
+      <c r="D53" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F53" t="s">
         <v>83</v>
       </c>
-      <c r="G53" s="6">
+      <c r="G53" s="5">
         <v>36</v>
       </c>
       <c r="H53">
         <v>22</v>
       </c>
-      <c r="I53" s="11" t="s">
+      <c r="I53" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="21" t="s">
+      <c r="A54" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="B54" s="20" t="s">
+      <c r="B54" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C54">
         <v>10</v>
       </c>
-      <c r="D54" s="15" t="s">
+      <c r="D54" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F54" t="s">
         <v>83</v>
       </c>
-      <c r="G54" s="6">
+      <c r="G54" s="5">
         <v>36</v>
       </c>
       <c r="H54">
         <v>25</v>
       </c>
-      <c r="I54" s="11" t="s">
+      <c r="I54" s="10" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="21" t="s">
+      <c r="A55" s="20" t="s">
         <v>80</v>
       </c>
-      <c r="B55" s="20" t="s">
+      <c r="B55" s="19" t="s">
         <v>10</v>
       </c>
       <c r="C55">
         <v>10</v>
       </c>
-      <c r="D55" s="15" t="s">
+      <c r="D55" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F55" t="s">
         <v>83</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55" s="5">
         <v>36</v>
       </c>
       <c r="H55">
         <v>25</v>
       </c>
-      <c r="I55" s="11" t="s">
+      <c r="I55" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2202,19 +2195,19 @@
       <c r="C56">
         <v>30</v>
       </c>
-      <c r="D56" s="15" t="s">
+      <c r="D56" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F56" t="s">
         <v>49</v>
       </c>
-      <c r="G56" s="6" t="s">
+      <c r="G56" s="5" t="s">
         <v>55</v>
       </c>
       <c r="H56">
         <v>0.15</v>
       </c>
-      <c r="I56" s="11" t="s">
+      <c r="I56" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2228,19 +2221,19 @@
       <c r="C57">
         <v>30</v>
       </c>
-      <c r="D57" s="15" t="s">
+      <c r="D57" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F57" t="s">
         <v>49</v>
       </c>
-      <c r="G57" s="6" t="s">
+      <c r="G57" s="5" t="s">
         <v>55</v>
       </c>
       <c r="H57">
         <v>0.15</v>
       </c>
-      <c r="I57" s="11" t="s">
+      <c r="I57" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2254,19 +2247,19 @@
       <c r="C58">
         <v>30</v>
       </c>
-      <c r="D58" s="15" t="s">
+      <c r="D58" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F58" t="s">
         <v>49</v>
       </c>
-      <c r="G58" s="6" t="s">
+      <c r="G58" s="5" t="s">
         <v>56</v>
       </c>
       <c r="H58">
         <v>0.15</v>
       </c>
-      <c r="I58" s="11" t="s">
+      <c r="I58" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2280,19 +2273,19 @@
       <c r="C59">
         <v>30</v>
       </c>
-      <c r="D59" s="15" t="s">
+      <c r="D59" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F59" t="s">
         <v>49</v>
       </c>
-      <c r="G59" s="6" t="s">
+      <c r="G59" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H59">
         <v>0.15</v>
       </c>
-      <c r="I59" s="11" t="s">
+      <c r="I59" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2306,19 +2299,19 @@
       <c r="C60">
         <v>30</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="D60" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F60" t="s">
         <v>49</v>
       </c>
-      <c r="G60" s="6" t="s">
+      <c r="G60" s="5" t="s">
         <v>57</v>
       </c>
       <c r="H60">
         <v>0.15</v>
       </c>
-      <c r="I60" s="11" t="s">
+      <c r="I60" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2332,19 +2325,19 @@
       <c r="C61">
         <v>20</v>
       </c>
-      <c r="D61" s="15" t="s">
+      <c r="D61" s="14" t="s">
         <v>12</v>
       </c>
       <c r="F61" t="s">
         <v>49</v>
       </c>
-      <c r="G61" s="6" t="s">
+      <c r="G61" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="H61" s="6">
-        <v>16</v>
-      </c>
-      <c r="I61" s="11" t="s">
+      <c r="H61" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="I61" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2358,19 +2351,19 @@
       <c r="C62">
         <v>40</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="D62" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="F62" s="5" t="s">
+      <c r="F62" s="15" t="s">
         <v>87</v>
       </c>
       <c r="G62">
         <v>4</v>
       </c>
-      <c r="H62">
-        <v>2</v>
-      </c>
-      <c r="I62" s="11" t="s">
+      <c r="H62" s="21" t="s">
+        <v>84</v>
+      </c>
+      <c r="I62" s="10" t="s">
         <v>32</v>
       </c>
     </row>
@@ -2384,7 +2377,7 @@
       <c r="C63">
         <v>70</v>
       </c>
-      <c r="D63" s="15" t="s">
+      <c r="D63" s="14" t="s">
         <v>89</v>
       </c>
       <c r="F63" t="s">
@@ -2396,7 +2389,7 @@
       <c r="H63">
         <v>3</v>
       </c>
-      <c r="I63" s="11" t="s">
+      <c r="I63" s="10" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Correções UML e Template da E3
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -737,7 +737,7 @@
   <dimension ref="A1:I63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H62" sqref="H62"/>
+      <selection activeCell="I66" sqref="I66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2360,8 +2360,8 @@
       <c r="G62">
         <v>4</v>
       </c>
-      <c r="H62" s="21" t="s">
-        <v>84</v>
+      <c r="H62" s="21">
+        <v>6</v>
       </c>
       <c r="I62" s="10" t="s">
         <v>32</v>

</xml_diff>

<commit_message>
Criação da E3 entre outros documentos
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="128">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Abrir uma conta no GitHub</t>
   </si>
   <si>
-    <t>Concluído</t>
-  </si>
-  <si>
     <t>https://github.com</t>
   </si>
   <si>
@@ -286,6 +283,123 @@
   </si>
   <si>
     <t>incompleto</t>
+  </si>
+  <si>
+    <t>Cria Iteração E3</t>
+  </si>
+  <si>
+    <t>Especificar o Caso de Uso Cad. Auxiliar_ Equipamento</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_ Equipamento</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Configuração das portas</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Chip GSM</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Operadora</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Plano do Chip</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Veículo Marca</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Veículo Modelo</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Veículo Cor</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Veículo  Ícone</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Ícone do Ponto</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Agenda</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Informativo</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Tipo de Manutenção</t>
+  </si>
+  <si>
+    <t>Criar modelo UML do Caso de uso/ Diagrama de Classe e Diagrama de Atividades da E3.</t>
+  </si>
+  <si>
+    <t>Completo</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_ Equipamento</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Tipo do equipamento</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Configuração das portas</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Chip GSM</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Operadora</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Plano do Chip</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Veículo Marca</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Veículo Modelo</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Veículo Cor</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Veículo  Ícone</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Ícone do Ponto</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Agenda</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Informativo</t>
+  </si>
+  <si>
+    <t>Criar Tela Cad. Auxiliar_Tipo de Manutenção</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_ Equipamento</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Tipo do equipamento</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Configuração das portas</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Chip GSM</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Operadora</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Plano do Chip</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Veículo Marca</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Veículo Modelo</t>
   </si>
 </sst>
 </file>
@@ -296,7 +410,7 @@
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -339,6 +453,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -385,13 +506,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,15 +524,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -437,11 +554,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+  <cellStyles count="3">
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Porcentagem" xfId="2" builtinId="5"/>
     <cellStyle name="Separador de milhares" xfId="1" builtinId="3"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -734,15 +851,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I63"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I66" sqref="I66"/>
+    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="90" workbookViewId="0">
+      <selection activeCell="K86" sqref="K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="53.85546875" customWidth="1"/>
+    <col min="1" max="1" width="66.85546875" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="3" width="9.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
@@ -791,25 +908,25 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="D2" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="H2">
         <v>0.5</v>
       </c>
-      <c r="I2" s="11" t="s">
-        <v>13</v>
+      <c r="I2" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -817,37 +934,37 @@
       <c r="C3">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="F3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>13</v>
-      </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="15" t="s">
+      <c r="A4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>9</v>
       </c>
       <c r="C4">
         <v>50</v>
       </c>
-      <c r="D4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>15</v>
+      <c r="D4" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>14</v>
       </c>
       <c r="G4" s="5">
         <v>48</v>
@@ -855,13 +972,13 @@
       <c r="H4" s="5">
         <v>22</v>
       </c>
-      <c r="I4" s="12" t="s">
-        <v>18</v>
+      <c r="I4" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
@@ -869,25 +986,25 @@
       <c r="C5">
         <v>165</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="F5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="18">
+        <v>24</v>
+      </c>
+      <c r="H5" s="12">
         <v>12</v>
       </c>
-      <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="21">
-        <v>24</v>
-      </c>
-      <c r="H5" s="15">
-        <v>12</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>18</v>
+      <c r="I5" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B6" t="s">
         <v>9</v>
@@ -895,11 +1012,11 @@
       <c r="C6">
         <v>180</v>
       </c>
-      <c r="D6" t="s">
-        <v>12</v>
+      <c r="D6" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5">
         <v>24</v>
@@ -907,13 +1024,13 @@
       <c r="H6">
         <v>8</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>18</v>
+      <c r="I6" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -921,11 +1038,11 @@
       <c r="C7">
         <v>160</v>
       </c>
-      <c r="D7" t="s">
-        <v>12</v>
+      <c r="D7" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G7" s="5">
         <v>36</v>
@@ -933,13 +1050,13 @@
       <c r="H7">
         <v>30</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>18</v>
+      <c r="I7" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -947,11 +1064,11 @@
       <c r="C8">
         <v>140</v>
       </c>
-      <c r="D8" t="s">
-        <v>12</v>
+      <c r="D8" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G8" s="5">
         <v>6</v>
@@ -959,13 +1076,13 @@
       <c r="H8">
         <v>4</v>
       </c>
-      <c r="I8" s="12" t="s">
-        <v>18</v>
+      <c r="I8" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="A9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
@@ -973,11 +1090,11 @@
       <c r="C9">
         <v>160</v>
       </c>
-      <c r="D9" t="s">
-        <v>12</v>
+      <c r="D9" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G9" s="5">
         <v>8</v>
@@ -985,13 +1102,13 @@
       <c r="H9">
         <v>4</v>
       </c>
-      <c r="I9" s="12" t="s">
-        <v>18</v>
+      <c r="I9" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
@@ -999,11 +1116,11 @@
       <c r="C10">
         <v>130</v>
       </c>
-      <c r="D10" t="s">
-        <v>12</v>
+      <c r="D10" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G10" s="5">
         <v>4</v>
@@ -1011,13 +1128,13 @@
       <c r="H10">
         <v>3</v>
       </c>
-      <c r="I10" s="12" t="s">
-        <v>18</v>
+      <c r="I10" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -1025,25 +1142,25 @@
       <c r="C11">
         <v>50</v>
       </c>
-      <c r="D11" t="s">
-        <v>12</v>
+      <c r="D11" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G11" s="5">
         <v>2</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="I11" s="10" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="15" t="s">
-        <v>50</v>
+      <c r="A12" s="12" t="s">
+        <v>49</v>
       </c>
       <c r="B12" t="s">
         <v>9</v>
@@ -1051,11 +1168,11 @@
       <c r="C12">
         <v>40</v>
       </c>
-      <c r="D12" t="s">
-        <v>12</v>
+      <c r="D12" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G12" s="5">
         <v>12</v>
@@ -1063,25 +1180,25 @@
       <c r="H12">
         <v>8</v>
       </c>
-      <c r="I12" s="10" t="s">
-        <v>32</v>
+      <c r="I12" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="25.5">
-      <c r="A13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="15" t="s">
+      <c r="A13" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C13">
         <v>220</v>
       </c>
-      <c r="D13" s="14" t="s">
-        <v>12</v>
+      <c r="D13" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G13" s="5">
         <v>24</v>
@@ -1089,13 +1206,13 @@
       <c r="H13">
         <v>24</v>
       </c>
-      <c r="I13" s="10" t="s">
-        <v>24</v>
+      <c r="I13" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B14" t="s">
         <v>9</v>
@@ -1103,25 +1220,25 @@
       <c r="C14">
         <v>40</v>
       </c>
-      <c r="D14" t="s">
-        <v>12</v>
+      <c r="D14" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G14" s="5">
         <v>72</v>
       </c>
-      <c r="H14" s="22">
+      <c r="H14" s="19">
         <v>36</v>
       </c>
-      <c r="I14" s="10" t="s">
-        <v>32</v>
+      <c r="I14" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="15" t="s">
-        <v>45</v>
+      <c r="A15" s="12" t="s">
+        <v>44</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
@@ -1129,11 +1246,11 @@
       <c r="C15">
         <v>110</v>
       </c>
-      <c r="D15" t="s">
-        <v>12</v>
+      <c r="D15" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G15" s="5">
         <v>36</v>
@@ -1141,13 +1258,13 @@
       <c r="H15">
         <v>36</v>
       </c>
-      <c r="I15" s="12" t="s">
-        <v>18</v>
+      <c r="I15" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
@@ -1155,25 +1272,25 @@
       <c r="C16">
         <v>20</v>
       </c>
-      <c r="D16" t="s">
-        <v>12</v>
+      <c r="D16" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G16" s="5">
         <v>36</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>36</v>
       </c>
-      <c r="I16" s="10" t="s">
-        <v>32</v>
+      <c r="I16" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="15" t="s">
-        <v>38</v>
+      <c r="A17" s="12" t="s">
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>9</v>
@@ -1181,11 +1298,11 @@
       <c r="C17">
         <v>80</v>
       </c>
-      <c r="D17" t="s">
-        <v>12</v>
+      <c r="D17" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G17" s="5">
         <v>4</v>
@@ -1193,13 +1310,13 @@
       <c r="H17">
         <v>3</v>
       </c>
-      <c r="I17" s="10" t="s">
-        <v>32</v>
+      <c r="I17" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
@@ -1207,25 +1324,25 @@
       <c r="C18">
         <v>60</v>
       </c>
-      <c r="D18" t="s">
-        <v>12</v>
+      <c r="D18" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G18" s="5">
         <v>24</v>
       </c>
-      <c r="H18" s="7">
+      <c r="H18" s="6">
         <v>12</v>
       </c>
-      <c r="I18" s="10" t="s">
-        <v>32</v>
+      <c r="I18" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="15" t="s">
-        <v>46</v>
+      <c r="A19" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
@@ -1233,11 +1350,11 @@
       <c r="C19">
         <v>110</v>
       </c>
-      <c r="D19" t="s">
-        <v>12</v>
+      <c r="D19" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G19" s="5">
         <v>4</v>
@@ -1245,13 +1362,13 @@
       <c r="H19">
         <v>2</v>
       </c>
-      <c r="I19" s="12" t="s">
-        <v>18</v>
+      <c r="I19" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
@@ -1259,25 +1376,25 @@
       <c r="C20">
         <v>20</v>
       </c>
-      <c r="D20" t="s">
-        <v>12</v>
+      <c r="D20" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G20" s="5">
         <v>36</v>
       </c>
-      <c r="H20" s="7">
+      <c r="H20" s="6">
         <v>36</v>
       </c>
-      <c r="I20" s="10" t="s">
-        <v>32</v>
+      <c r="I20" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="15" t="s">
-        <v>44</v>
+      <c r="A21" s="12" t="s">
+        <v>43</v>
       </c>
       <c r="B21" t="s">
         <v>9</v>
@@ -1285,11 +1402,11 @@
       <c r="C21">
         <v>60</v>
       </c>
-      <c r="D21" t="s">
-        <v>12</v>
+      <c r="D21" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G21" s="5">
         <v>6</v>
@@ -1297,13 +1414,13 @@
       <c r="H21">
         <v>5</v>
       </c>
-      <c r="I21" s="10" t="s">
-        <v>32</v>
+      <c r="I21" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
         <v>9</v>
@@ -1311,11 +1428,11 @@
       <c r="C22">
         <v>30</v>
       </c>
-      <c r="D22" t="s">
-        <v>12</v>
+      <c r="D22" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G22" s="5">
         <v>2</v>
@@ -1323,13 +1440,13 @@
       <c r="H22">
         <v>1</v>
       </c>
-      <c r="I22" s="10" t="s">
-        <v>32</v>
+      <c r="I22" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B23" t="s">
         <v>9</v>
@@ -1337,11 +1454,11 @@
       <c r="C23">
         <v>30</v>
       </c>
-      <c r="D23" t="s">
-        <v>12</v>
+      <c r="D23" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F23" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G23" s="5">
         <v>2</v>
@@ -1349,13 +1466,13 @@
       <c r="H23">
         <v>2</v>
       </c>
-      <c r="I23" s="10" t="s">
-        <v>32</v>
+      <c r="I23" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B24" t="s">
         <v>9</v>
@@ -1363,11 +1480,11 @@
       <c r="C24">
         <v>30</v>
       </c>
-      <c r="D24" t="s">
-        <v>12</v>
+      <c r="D24" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G24" s="5">
         <v>2</v>
@@ -1375,13 +1492,13 @@
       <c r="H24">
         <v>1</v>
       </c>
-      <c r="I24" s="10" t="s">
-        <v>32</v>
+      <c r="I24" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
@@ -1389,11 +1506,11 @@
       <c r="C25">
         <v>30</v>
       </c>
-      <c r="D25" t="s">
-        <v>12</v>
+      <c r="D25" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G25" s="5">
         <v>1</v>
@@ -1401,13 +1518,13 @@
       <c r="H25">
         <v>1</v>
       </c>
-      <c r="I25" s="10" t="s">
-        <v>32</v>
+      <c r="I25" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
         <v>9</v>
@@ -1415,11 +1532,11 @@
       <c r="C26">
         <v>30</v>
       </c>
-      <c r="D26" t="s">
-        <v>12</v>
+      <c r="D26" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G26" s="5">
         <v>2</v>
@@ -1427,13 +1544,13 @@
       <c r="H26">
         <v>1</v>
       </c>
-      <c r="I26" s="10" t="s">
-        <v>32</v>
+      <c r="I26" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
         <v>9</v>
@@ -1441,11 +1558,11 @@
       <c r="C27">
         <v>30</v>
       </c>
-      <c r="D27" s="9" t="s">
-        <v>12</v>
+      <c r="D27" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G27" s="5">
         <v>2</v>
@@ -1453,25 +1570,25 @@
       <c r="H27">
         <v>1</v>
       </c>
-      <c r="I27" s="10" t="s">
-        <v>32</v>
+      <c r="I27" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28">
         <v>60</v>
       </c>
-      <c r="D28" s="8" t="s">
-        <v>12</v>
+      <c r="D28" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G28" s="5">
         <v>1</v>
@@ -1479,13 +1596,13 @@
       <c r="H28">
         <v>1</v>
       </c>
-      <c r="I28" s="10" t="s">
-        <v>32</v>
+      <c r="I28" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:9">
-      <c r="A29" s="13" t="s">
-        <v>47</v>
+      <c r="A29" s="10" t="s">
+        <v>46</v>
       </c>
       <c r="B29" t="s">
         <v>9</v>
@@ -1493,11 +1610,11 @@
       <c r="C29">
         <v>100</v>
       </c>
-      <c r="D29" s="6" t="s">
-        <v>12</v>
+      <c r="D29" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G29" s="5">
         <v>48</v>
@@ -1505,13 +1622,13 @@
       <c r="H29">
         <v>42</v>
       </c>
-      <c r="I29" s="10" t="s">
-        <v>32</v>
+      <c r="I29" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B30" t="s">
         <v>10</v>
@@ -1519,11 +1636,11 @@
       <c r="C30">
         <v>100</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>12</v>
+      <c r="D30" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G30" s="5">
         <v>16</v>
@@ -1531,25 +1648,25 @@
       <c r="H30" s="5">
         <v>12</v>
       </c>
-      <c r="I30" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="51">
-      <c r="A31" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B31" s="15" t="s">
+      <c r="I30" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="38.25">
+      <c r="A31" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B31" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C31">
         <v>440</v>
       </c>
-      <c r="D31" s="14" t="s">
-        <v>12</v>
+      <c r="D31" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="G31" s="5">
         <v>48</v>
@@ -1557,13 +1674,13 @@
       <c r="H31">
         <v>36</v>
       </c>
-      <c r="I31" s="10" t="s">
-        <v>24</v>
+      <c r="I31" s="7" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:9">
       <c r="A32" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" t="s">
         <v>9</v>
@@ -1571,25 +1688,25 @@
       <c r="C32">
         <v>120</v>
       </c>
-      <c r="D32" s="14" t="s">
-        <v>12</v>
+      <c r="D32" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G32" s="5">
         <v>4</v>
       </c>
-      <c r="H32" s="17">
+      <c r="H32" s="14">
         <v>2</v>
       </c>
-      <c r="I32" s="10" t="s">
-        <v>32</v>
+      <c r="I32" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:9">
-      <c r="A33" s="15" t="s">
-        <v>52</v>
+      <c r="A33" s="12" t="s">
+        <v>51</v>
       </c>
       <c r="B33" t="s">
         <v>9</v>
@@ -1597,11 +1714,11 @@
       <c r="C33">
         <v>60</v>
       </c>
-      <c r="D33" s="14" t="s">
-        <v>12</v>
+      <c r="D33" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F33" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G33" s="5">
         <v>1</v>
@@ -1609,13 +1726,13 @@
       <c r="H33">
         <v>1</v>
       </c>
-      <c r="I33" s="12" t="s">
-        <v>18</v>
+      <c r="I33" s="9" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:9">
       <c r="A34" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
@@ -1623,25 +1740,25 @@
       <c r="C34">
         <v>10</v>
       </c>
-      <c r="D34" s="14" t="s">
-        <v>12</v>
+      <c r="D34" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G34" s="5">
         <v>1</v>
       </c>
-      <c r="H34" s="16">
+      <c r="H34" s="13">
         <v>1</v>
       </c>
-      <c r="I34" s="10" t="s">
-        <v>32</v>
+      <c r="I34" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:9">
-      <c r="A35" s="15" t="s">
-        <v>54</v>
+      <c r="A35" s="12" t="s">
+        <v>53</v>
       </c>
       <c r="B35" t="s">
         <v>9</v>
@@ -1649,11 +1766,11 @@
       <c r="C35">
         <v>80</v>
       </c>
-      <c r="D35" s="14" t="s">
-        <v>12</v>
+      <c r="D35" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F35" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G35" s="5">
         <v>4</v>
@@ -1661,25 +1778,25 @@
       <c r="H35">
         <v>1.32</v>
       </c>
-      <c r="I35" s="10" t="s">
-        <v>32</v>
+      <c r="I35" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:9">
-      <c r="A36" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B36" s="19" t="s">
+      <c r="A36" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B36" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C36">
         <v>80</v>
       </c>
-      <c r="D36" s="14" t="s">
-        <v>12</v>
+      <c r="D36" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G36" s="5">
         <v>4</v>
@@ -1687,25 +1804,25 @@
       <c r="H36">
         <v>2</v>
       </c>
-      <c r="I36" s="10" t="s">
-        <v>32</v>
+      <c r="I36" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:9">
-      <c r="A37" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B37" s="19" t="s">
+      <c r="A37" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B37" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C37">
         <v>80</v>
       </c>
-      <c r="D37" s="14" t="s">
-        <v>12</v>
+      <c r="D37" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G37" s="5">
         <v>4</v>
@@ -1713,25 +1830,25 @@
       <c r="H37">
         <v>2</v>
       </c>
-      <c r="I37" s="10" t="s">
-        <v>32</v>
+      <c r="I37" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:9">
-      <c r="A38" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="B38" s="19" t="s">
+      <c r="A38" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="B38" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C38">
         <v>80</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>12</v>
+      <c r="D38" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G38" s="5">
         <v>4</v>
@@ -1739,25 +1856,25 @@
       <c r="H38">
         <v>3</v>
       </c>
-      <c r="I38" s="10" t="s">
-        <v>32</v>
+      <c r="I38" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="1:9">
-      <c r="A39" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="B39" s="19" t="s">
+      <c r="A39" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="B39" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C39">
         <v>80</v>
       </c>
-      <c r="D39" s="14" t="s">
-        <v>12</v>
+      <c r="D39" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G39" s="5">
         <v>4</v>
@@ -1765,25 +1882,25 @@
       <c r="H39">
         <v>2</v>
       </c>
-      <c r="I39" s="10" t="s">
-        <v>32</v>
+      <c r="I39" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="40" spans="1:9">
-      <c r="A40" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="B40" s="19" t="s">
+      <c r="A40" s="15" t="s">
+        <v>64</v>
+      </c>
+      <c r="B40" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C40">
         <v>80</v>
       </c>
-      <c r="D40" s="14" t="s">
-        <v>12</v>
+      <c r="D40" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G40" s="5">
         <v>4</v>
@@ -1791,25 +1908,25 @@
       <c r="H40">
         <v>3</v>
       </c>
-      <c r="I40" s="10" t="s">
-        <v>32</v>
+      <c r="I40" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:9">
-      <c r="A41" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="B41" s="19" t="s">
+      <c r="A41" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="B41" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C41">
         <v>120</v>
       </c>
-      <c r="D41" s="14" t="s">
-        <v>12</v>
+      <c r="D41" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F41" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G41" s="5">
         <v>36</v>
@@ -1817,25 +1934,25 @@
       <c r="H41">
         <v>24</v>
       </c>
-      <c r="I41" s="10" t="s">
-        <v>32</v>
+      <c r="I41" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:9">
-      <c r="A42" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="19" t="s">
+      <c r="A42" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="B42" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C42">
         <v>120</v>
       </c>
-      <c r="D42" s="14" t="s">
-        <v>12</v>
+      <c r="D42" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F42" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G42" s="5">
         <v>24</v>
@@ -1843,25 +1960,25 @@
       <c r="H42">
         <v>12</v>
       </c>
-      <c r="I42" s="10" t="s">
-        <v>32</v>
+      <c r="I42" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="43" spans="1:9">
-      <c r="A43" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="19" t="s">
+      <c r="A43" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="B43" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C43">
         <v>120</v>
       </c>
-      <c r="D43" s="14" t="s">
-        <v>12</v>
+      <c r="D43" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F43" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G43" s="5">
         <v>24</v>
@@ -1869,25 +1986,25 @@
       <c r="H43">
         <v>8</v>
       </c>
-      <c r="I43" s="10" t="s">
-        <v>32</v>
+      <c r="I43" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:9">
-      <c r="A44" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="B44" s="19" t="s">
+      <c r="A44" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B44" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C44">
         <v>120</v>
       </c>
-      <c r="D44" s="14" t="s">
-        <v>12</v>
+      <c r="D44" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F44" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G44" s="5">
         <v>24</v>
@@ -1895,25 +2012,25 @@
       <c r="H44">
         <v>8</v>
       </c>
-      <c r="I44" s="10" t="s">
-        <v>32</v>
+      <c r="I44" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="45" spans="1:9">
-      <c r="A45" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="B45" s="19" t="s">
+      <c r="A45" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C45">
         <v>120</v>
       </c>
-      <c r="D45" s="14" t="s">
-        <v>12</v>
+      <c r="D45" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F45" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G45" s="5">
         <v>24</v>
@@ -1921,155 +2038,155 @@
       <c r="H45">
         <v>6</v>
       </c>
-      <c r="I45" s="10" t="s">
-        <v>32</v>
+      <c r="I45" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="46" spans="1:9">
-      <c r="A46" s="20" t="s">
-        <v>71</v>
-      </c>
-      <c r="B46" s="19" t="s">
+      <c r="A46" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C46">
         <v>60</v>
       </c>
-      <c r="D46" s="14" t="s">
-        <v>12</v>
+      <c r="D46" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F46" t="s">
+        <v>82</v>
+      </c>
+      <c r="G46" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G46" s="5" t="s">
+      <c r="H46" s="18" t="s">
         <v>84</v>
       </c>
-      <c r="H46" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="I46" s="10" t="s">
-        <v>32</v>
+      <c r="I46" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="47" spans="1:9">
-      <c r="A47" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B47" s="19" t="s">
+      <c r="A47" s="17" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C47">
         <v>60</v>
       </c>
-      <c r="D47" s="14" t="s">
-        <v>12</v>
+      <c r="D47" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F47" t="s">
+        <v>82</v>
+      </c>
+      <c r="G47" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G47" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H47" s="15">
+      <c r="H47" s="12">
         <v>2</v>
       </c>
-      <c r="I47" s="10" t="s">
-        <v>32</v>
+      <c r="I47" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="48" spans="1:9">
-      <c r="A48" s="20" t="s">
-        <v>73</v>
-      </c>
-      <c r="B48" s="19" t="s">
+      <c r="A48" s="17" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C48">
         <v>60</v>
       </c>
-      <c r="D48" s="14" t="s">
-        <v>12</v>
+      <c r="D48" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F48" t="s">
+        <v>82</v>
+      </c>
+      <c r="G48" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G48" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H48" s="21">
+      <c r="H48" s="18">
         <v>2.5</v>
       </c>
-      <c r="I48" s="10" t="s">
-        <v>32</v>
+      <c r="I48" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="B49" s="19" t="s">
+      <c r="A49" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C49">
         <v>60</v>
       </c>
-      <c r="D49" s="14" t="s">
-        <v>12</v>
+      <c r="D49" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F49" t="s">
+        <v>82</v>
+      </c>
+      <c r="G49" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G49" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H49" s="21">
+      <c r="H49" s="18">
         <v>1.7</v>
       </c>
-      <c r="I49" s="10" t="s">
-        <v>32</v>
+      <c r="I49" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="20" t="s">
-        <v>75</v>
-      </c>
-      <c r="B50" s="19" t="s">
+      <c r="A50" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B50" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C50">
         <v>60</v>
       </c>
-      <c r="D50" s="14" t="s">
-        <v>12</v>
+      <c r="D50" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F50" t="s">
+        <v>82</v>
+      </c>
+      <c r="G50" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="G50" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="H50" s="15">
+      <c r="H50" s="12">
         <v>3</v>
       </c>
-      <c r="I50" s="10" t="s">
-        <v>32</v>
+      <c r="I50" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="20" t="s">
-        <v>76</v>
-      </c>
-      <c r="B51" s="19" t="s">
+      <c r="A51" s="17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B51" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C51">
         <v>10</v>
       </c>
-      <c r="D51" s="14" t="s">
-        <v>12</v>
+      <c r="D51" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F51" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G51" s="5">
         <v>36</v>
@@ -2077,25 +2194,25 @@
       <c r="H51">
         <v>32</v>
       </c>
-      <c r="I51" s="10" t="s">
-        <v>32</v>
+      <c r="I51" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="B52" s="19" t="s">
+      <c r="A52" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="B52" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C52">
         <v>10</v>
       </c>
-      <c r="D52" s="14" t="s">
-        <v>12</v>
+      <c r="D52" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F52" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G52" s="5">
         <v>36</v>
@@ -2103,25 +2220,25 @@
       <c r="H52">
         <v>18</v>
       </c>
-      <c r="I52" s="10" t="s">
-        <v>32</v>
+      <c r="I52" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B53" s="19" t="s">
+      <c r="A53" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B53" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C53">
         <v>10</v>
       </c>
-      <c r="D53" s="14" t="s">
-        <v>12</v>
+      <c r="D53" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F53" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G53" s="5">
         <v>36</v>
@@ -2129,25 +2246,25 @@
       <c r="H53">
         <v>22</v>
       </c>
-      <c r="I53" s="10" t="s">
-        <v>32</v>
+      <c r="I53" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="B54" s="19" t="s">
+      <c r="A54" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B54" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C54">
         <v>10</v>
       </c>
-      <c r="D54" s="14" t="s">
-        <v>12</v>
+      <c r="D54" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G54" s="5">
         <v>36</v>
@@ -2155,25 +2272,25 @@
       <c r="H54">
         <v>25</v>
       </c>
-      <c r="I54" s="10" t="s">
-        <v>32</v>
+      <c r="I54" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="B55" s="19" t="s">
+      <c r="A55" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B55" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C55">
         <v>10</v>
       </c>
-      <c r="D55" s="14" t="s">
-        <v>12</v>
+      <c r="D55" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F55" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G55" s="5">
         <v>36</v>
@@ -2181,13 +2298,13 @@
       <c r="H55">
         <v>25</v>
       </c>
-      <c r="I55" s="10" t="s">
-        <v>32</v>
+      <c r="I55" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B56" t="s">
         <v>9</v>
@@ -2195,25 +2312,25 @@
       <c r="C56">
         <v>30</v>
       </c>
-      <c r="D56" s="14" t="s">
-        <v>12</v>
+      <c r="D56" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F56" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H56">
         <v>0.15</v>
       </c>
-      <c r="I56" s="10" t="s">
-        <v>32</v>
+      <c r="I56" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B57" t="s">
         <v>9</v>
@@ -2221,25 +2338,25 @@
       <c r="C57">
         <v>30</v>
       </c>
-      <c r="D57" s="14" t="s">
-        <v>12</v>
+      <c r="D57" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F57" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H57">
         <v>0.15</v>
       </c>
-      <c r="I57" s="10" t="s">
-        <v>32</v>
+      <c r="I57" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B58" t="s">
         <v>9</v>
@@ -2247,25 +2364,25 @@
       <c r="C58">
         <v>30</v>
       </c>
-      <c r="D58" s="14" t="s">
-        <v>12</v>
+      <c r="D58" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H58">
         <v>0.15</v>
       </c>
-      <c r="I58" s="10" t="s">
-        <v>32</v>
+      <c r="I58" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B59" t="s">
         <v>9</v>
@@ -2273,51 +2390,51 @@
       <c r="C59">
         <v>30</v>
       </c>
-      <c r="D59" s="14" t="s">
-        <v>12</v>
+      <c r="D59" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F59" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H59">
         <v>0.15</v>
       </c>
-      <c r="I59" s="10" t="s">
-        <v>32</v>
+      <c r="I59" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C60">
         <v>30</v>
       </c>
-      <c r="D60" s="14" t="s">
-        <v>12</v>
+      <c r="D60" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H60">
         <v>0.15</v>
       </c>
-      <c r="I60" s="10" t="s">
-        <v>32</v>
+      <c r="I60" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
         <v>9</v>
@@ -2325,25 +2442,25 @@
       <c r="C61">
         <v>20</v>
       </c>
-      <c r="D61" s="14" t="s">
-        <v>12</v>
+      <c r="D61" s="12" t="s">
+        <v>105</v>
       </c>
       <c r="F61" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H61" s="21" t="s">
-        <v>85</v>
-      </c>
-      <c r="I61" s="10" t="s">
-        <v>32</v>
+        <v>59</v>
+      </c>
+      <c r="H61" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="I61" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B62" t="s">
         <v>10</v>
@@ -2351,25 +2468,25 @@
       <c r="C62">
         <v>40</v>
       </c>
-      <c r="D62" s="14" t="s">
-        <v>82</v>
-      </c>
-      <c r="F62" s="15" t="s">
-        <v>87</v>
+      <c r="D62" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="F62" s="12" t="s">
+        <v>86</v>
       </c>
       <c r="G62">
         <v>4</v>
       </c>
-      <c r="H62" s="21">
+      <c r="H62" s="18">
         <v>6</v>
       </c>
-      <c r="I62" s="10" t="s">
-        <v>32</v>
+      <c r="I62" s="7" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B63" t="s">
         <v>10</v>
@@ -2377,11 +2494,11 @@
       <c r="C63">
         <v>70</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>89</v>
+      <c r="D63" s="11" t="s">
+        <v>88</v>
       </c>
       <c r="F63" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G63">
         <v>4</v>
@@ -2389,9 +2506,916 @@
       <c r="H63">
         <v>3</v>
       </c>
-      <c r="I63" s="10" t="s">
-        <v>32</v>
-      </c>
+      <c r="I63" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="B65" t="s">
+        <v>9</v>
+      </c>
+      <c r="C65">
+        <v>60</v>
+      </c>
+      <c r="D65" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="F65" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G65" s="5">
+        <v>1</v>
+      </c>
+      <c r="H65">
+        <v>1</v>
+      </c>
+      <c r="I65" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="15" t="s">
+        <v>91</v>
+      </c>
+      <c r="B66" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C66">
+        <v>60</v>
+      </c>
+      <c r="D66" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F66" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G66" s="5">
+        <v>1</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+      <c r="I66" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="15" t="s">
+        <v>92</v>
+      </c>
+      <c r="B67" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C67">
+        <v>60</v>
+      </c>
+      <c r="D67" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F67" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G67" s="5">
+        <v>1</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
+      <c r="A68" s="15" t="s">
+        <v>93</v>
+      </c>
+      <c r="B68" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C68">
+        <v>60</v>
+      </c>
+      <c r="D68" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F68" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G68" s="5">
+        <v>1</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+      <c r="I68" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
+      <c r="A69" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="B69" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C69">
+        <v>60</v>
+      </c>
+      <c r="D69" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F69" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G69" s="5">
+        <v>1</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
+      <c r="A70" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C70">
+        <v>60</v>
+      </c>
+      <c r="D70" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F70" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G70" s="5">
+        <v>1</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+      <c r="I70" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
+      <c r="A71" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B71" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C71">
+        <v>60</v>
+      </c>
+      <c r="D71" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F71" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G71" s="5">
+        <v>1</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+      <c r="I71" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
+      <c r="A72" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B72" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C72">
+        <v>60</v>
+      </c>
+      <c r="D72" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F72" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G72" s="5">
+        <v>1</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
+      <c r="A73" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B73" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C73">
+        <v>60</v>
+      </c>
+      <c r="D73" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F73" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G73" s="5">
+        <v>1</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+      <c r="I73" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
+      <c r="A74" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="B74" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C74">
+        <v>60</v>
+      </c>
+      <c r="D74" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F74" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G74" s="5">
+        <v>1</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
+      <c r="A75" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B75" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C75">
+        <v>60</v>
+      </c>
+      <c r="D75" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F75" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G75" s="5">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
+      <c r="A76" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="B76" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C76">
+        <v>60</v>
+      </c>
+      <c r="D76" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F76" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G76" s="5">
+        <v>1</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
+      <c r="A77" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="B77" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C77">
+        <v>60</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F77" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G77" s="5">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
+      <c r="A78" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="B78" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C78">
+        <v>60</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F78" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G78" s="5">
+        <v>1</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" ht="26.25" customHeight="1">
+      <c r="A79" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B79" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C79">
+        <v>440</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F79" t="s">
+        <v>14</v>
+      </c>
+      <c r="G79" s="5">
+        <v>48</v>
+      </c>
+      <c r="H79">
+        <v>4</v>
+      </c>
+      <c r="I79" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
+      <c r="A80" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="B80" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C80">
+        <v>50</v>
+      </c>
+      <c r="D80" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F80" t="s">
+        <v>14</v>
+      </c>
+      <c r="G80" s="5">
+        <v>4</v>
+      </c>
+      <c r="I80" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
+      <c r="A81" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C81">
+        <v>50</v>
+      </c>
+      <c r="D81" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F81" t="s">
+        <v>14</v>
+      </c>
+      <c r="G81" s="5">
+        <v>4</v>
+      </c>
+      <c r="I81" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
+      <c r="A82" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="B82" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C82">
+        <v>50</v>
+      </c>
+      <c r="D82" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F82" t="s">
+        <v>14</v>
+      </c>
+      <c r="G82" s="5">
+        <v>4</v>
+      </c>
+      <c r="I82" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
+      <c r="A83" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="B83" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C83">
+        <v>50</v>
+      </c>
+      <c r="D83" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F83" t="s">
+        <v>14</v>
+      </c>
+      <c r="G83" s="5">
+        <v>4</v>
+      </c>
+      <c r="I83" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
+      <c r="A84" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B84" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C84">
+        <v>50</v>
+      </c>
+      <c r="D84" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" t="s">
+        <v>14</v>
+      </c>
+      <c r="G84" s="5">
+        <v>4</v>
+      </c>
+      <c r="I84" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
+      <c r="A85" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="B85" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C85">
+        <v>50</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F85" t="s">
+        <v>14</v>
+      </c>
+      <c r="G85" s="5">
+        <v>4</v>
+      </c>
+      <c r="I85" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
+      <c r="A86" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="B86" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C86">
+        <v>50</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F86" t="s">
+        <v>14</v>
+      </c>
+      <c r="G86" s="5">
+        <v>4</v>
+      </c>
+      <c r="I86" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
+      <c r="A87" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B87" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C87">
+        <v>50</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F87" t="s">
+        <v>14</v>
+      </c>
+      <c r="G87" s="5">
+        <v>4</v>
+      </c>
+      <c r="I87" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
+      <c r="A88" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="B88" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C88">
+        <v>50</v>
+      </c>
+      <c r="D88" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F88" t="s">
+        <v>14</v>
+      </c>
+      <c r="G88" s="5">
+        <v>4</v>
+      </c>
+      <c r="I88" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
+      <c r="A89" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C89">
+        <v>50</v>
+      </c>
+      <c r="D89" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F89" t="s">
+        <v>14</v>
+      </c>
+      <c r="G89" s="5">
+        <v>4</v>
+      </c>
+      <c r="I89" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
+      <c r="A90" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C90">
+        <v>50</v>
+      </c>
+      <c r="D90" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F90" t="s">
+        <v>14</v>
+      </c>
+      <c r="G90" s="5">
+        <v>4</v>
+      </c>
+      <c r="I90" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
+      <c r="A91" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="B91" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C91">
+        <v>50</v>
+      </c>
+      <c r="D91" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F91" t="s">
+        <v>14</v>
+      </c>
+      <c r="G91" s="5">
+        <v>4</v>
+      </c>
+      <c r="I91" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C92">
+        <v>50</v>
+      </c>
+      <c r="D92" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F92" t="s">
+        <v>14</v>
+      </c>
+      <c r="G92" s="5">
+        <v>4</v>
+      </c>
+      <c r="I92" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B93" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C93">
+        <v>50</v>
+      </c>
+      <c r="D93" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F93" t="s">
+        <v>14</v>
+      </c>
+      <c r="G93" s="5">
+        <v>4</v>
+      </c>
+      <c r="I93" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B94" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C94">
+        <v>30</v>
+      </c>
+      <c r="D94" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F94" t="s">
+        <v>14</v>
+      </c>
+      <c r="G94" s="5">
+        <v>2</v>
+      </c>
+      <c r="I94" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B95" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C95">
+        <v>30</v>
+      </c>
+      <c r="D95" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F95" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G95" s="5">
+        <v>2</v>
+      </c>
+      <c r="I95" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="B96" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C96">
+        <v>30</v>
+      </c>
+      <c r="D96" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F96" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G96" s="5">
+        <v>2</v>
+      </c>
+      <c r="I96" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="B97" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C97">
+        <v>30</v>
+      </c>
+      <c r="D97" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F97" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G97" s="5">
+        <v>2</v>
+      </c>
+      <c r="I97" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="B98" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C98">
+        <v>30</v>
+      </c>
+      <c r="D98" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F98" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G98" s="5">
+        <v>2</v>
+      </c>
+      <c r="I98" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="B99" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C99">
+        <v>30</v>
+      </c>
+      <c r="D99" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F99" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G99" s="5">
+        <v>2</v>
+      </c>
+      <c r="I99" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="B100" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C100">
+        <v>30</v>
+      </c>
+      <c r="D100" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F100" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G100" s="5">
+        <v>2</v>
+      </c>
+      <c r="I100" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="B101" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C101">
+        <v>30</v>
+      </c>
+      <c r="D101" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F101" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G101" s="5">
+        <v>2</v>
+      </c>
+      <c r="I101" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="G102" s="5"/>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="G103" s="5"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -2441,9 +3465,38 @@
     <hyperlink ref="I62" r:id="rId43"/>
     <hyperlink ref="I63" r:id="rId44"/>
     <hyperlink ref="I35:I55" r:id="rId45" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I65" r:id="rId46"/>
+    <hyperlink ref="I65:I70" r:id="rId47" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I69" r:id="rId48"/>
+    <hyperlink ref="I73" r:id="rId49"/>
+    <hyperlink ref="I77" r:id="rId50"/>
+    <hyperlink ref="I69:I78" r:id="rId51" display="https://github.com/valtervasconcelos/Projeto_de_Software_1"/>
+    <hyperlink ref="I79" r:id="rId52"/>
+    <hyperlink ref="I80" r:id="rId53"/>
+    <hyperlink ref="I81" r:id="rId54"/>
+    <hyperlink ref="I82" r:id="rId55"/>
+    <hyperlink ref="I84" r:id="rId56"/>
+    <hyperlink ref="I86" r:id="rId57"/>
+    <hyperlink ref="I88" r:id="rId58"/>
+    <hyperlink ref="I90" r:id="rId59"/>
+    <hyperlink ref="I92" r:id="rId60"/>
+    <hyperlink ref="I94" r:id="rId61"/>
+    <hyperlink ref="I96" r:id="rId62"/>
+    <hyperlink ref="I98" r:id="rId63"/>
+    <hyperlink ref="I100" r:id="rId64"/>
+    <hyperlink ref="I83" r:id="rId65"/>
+    <hyperlink ref="I85" r:id="rId66"/>
+    <hyperlink ref="I87" r:id="rId67"/>
+    <hyperlink ref="I89" r:id="rId68"/>
+    <hyperlink ref="I91" r:id="rId69"/>
+    <hyperlink ref="I93" r:id="rId70"/>
+    <hyperlink ref="I95" r:id="rId71"/>
+    <hyperlink ref="I97" r:id="rId72"/>
+    <hyperlink ref="I99" r:id="rId73"/>
+    <hyperlink ref="I101" r:id="rId74"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId46"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId75"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Atualização da Iteração E3
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="128">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C73" zoomScale="90" workbookViewId="0">
-      <selection activeCell="K86" sqref="K86"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H65" sqref="H65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2513,6 +2513,24 @@
     <row r="64" spans="1:9">
       <c r="A64" t="s">
         <v>89</v>
+      </c>
+      <c r="B64" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64">
+        <v>100</v>
+      </c>
+      <c r="D64" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="F64" t="s">
+        <v>86</v>
+      </c>
+      <c r="G64">
+        <v>12</v>
+      </c>
+      <c r="H64">
+        <v>6</v>
       </c>
     </row>
     <row r="65" spans="1:9">

</xml_diff>

<commit_message>
Nova Espec. Caso de Uso, entre outros.
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="134">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -291,9 +291,6 @@
     <t>Especificar o Caso de Uso Cad. Auxiliar_ Equipamento</t>
   </si>
   <si>
-    <t>Especificar o caso de uso Cad. Auxiliar_ Equipamento</t>
-  </si>
-  <si>
     <t>Especificar o caso de uso Cad. Auxiliar_Configuração das portas</t>
   </si>
   <si>
@@ -400,6 +397,27 @@
   </si>
   <si>
     <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Veículo Modelo</t>
+  </si>
+  <si>
+    <t>Especificar o caso de uso Cad. Auxiliar_Tipo do Equipamento</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Veículo Cor</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Veículo  Ícone</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Ícone do Ponto</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Agenda</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Informativo</t>
+  </si>
+  <si>
+    <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Tipo de Manutenção</t>
   </si>
 </sst>
 </file>
@@ -851,10 +869,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H65" sqref="H65"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="90" workbookViewId="0">
+      <selection activeCell="A113" sqref="A113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -909,7 +927,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F2" t="s">
         <v>14</v>
@@ -935,7 +953,7 @@
         <v>20</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
@@ -961,7 +979,7 @@
         <v>50</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F4" s="12" t="s">
         <v>14</v>
@@ -987,7 +1005,7 @@
         <v>165</v>
       </c>
       <c r="D5" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" t="s">
         <v>14</v>
@@ -1013,7 +1031,7 @@
         <v>180</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
@@ -1039,7 +1057,7 @@
         <v>160</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F7" t="s">
         <v>14</v>
@@ -1065,7 +1083,7 @@
         <v>140</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F8" t="s">
         <v>14</v>
@@ -1091,7 +1109,7 @@
         <v>160</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F9" t="s">
         <v>14</v>
@@ -1117,7 +1135,7 @@
         <v>130</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F10" t="s">
         <v>14</v>
@@ -1143,7 +1161,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F11" t="s">
         <v>14</v>
@@ -1169,7 +1187,7 @@
         <v>40</v>
       </c>
       <c r="D12" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F12" t="s">
         <v>14</v>
@@ -1195,7 +1213,7 @@
         <v>220</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F13" t="s">
         <v>14</v>
@@ -1221,7 +1239,7 @@
         <v>40</v>
       </c>
       <c r="D14" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F14" t="s">
         <v>14</v>
@@ -1247,7 +1265,7 @@
         <v>110</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F15" t="s">
         <v>14</v>
@@ -1273,7 +1291,7 @@
         <v>20</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
@@ -1299,7 +1317,7 @@
         <v>80</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F17" t="s">
         <v>14</v>
@@ -1325,7 +1343,7 @@
         <v>60</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F18" t="s">
         <v>14</v>
@@ -1351,7 +1369,7 @@
         <v>110</v>
       </c>
       <c r="D19" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F19" t="s">
         <v>14</v>
@@ -1377,7 +1395,7 @@
         <v>20</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
@@ -1403,7 +1421,7 @@
         <v>60</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F21" t="s">
         <v>14</v>
@@ -1429,7 +1447,7 @@
         <v>30</v>
       </c>
       <c r="D22" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F22" t="s">
         <v>14</v>
@@ -1455,7 +1473,7 @@
         <v>30</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F23" t="s">
         <v>14</v>
@@ -1481,7 +1499,7 @@
         <v>30</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
@@ -1507,7 +1525,7 @@
         <v>30</v>
       </c>
       <c r="D25" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F25" t="s">
         <v>14</v>
@@ -1533,7 +1551,7 @@
         <v>30</v>
       </c>
       <c r="D26" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F26" t="s">
         <v>14</v>
@@ -1559,7 +1577,7 @@
         <v>30</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F27" t="s">
         <v>14</v>
@@ -1585,7 +1603,7 @@
         <v>60</v>
       </c>
       <c r="D28" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F28" t="s">
         <v>14</v>
@@ -1611,7 +1629,7 @@
         <v>100</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F29" t="s">
         <v>14</v>
@@ -1637,7 +1655,7 @@
         <v>100</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F30" t="s">
         <v>48</v>
@@ -1663,7 +1681,7 @@
         <v>440</v>
       </c>
       <c r="D31" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F31" t="s">
         <v>14</v>
@@ -1689,7 +1707,7 @@
         <v>120</v>
       </c>
       <c r="D32" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F32" t="s">
         <v>48</v>
@@ -1715,7 +1733,7 @@
         <v>60</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F33" t="s">
         <v>48</v>
@@ -1741,7 +1759,7 @@
         <v>10</v>
       </c>
       <c r="D34" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F34" t="s">
         <v>48</v>
@@ -1767,7 +1785,7 @@
         <v>80</v>
       </c>
       <c r="D35" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F35" t="s">
         <v>48</v>
@@ -1793,7 +1811,7 @@
         <v>80</v>
       </c>
       <c r="D36" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F36" t="s">
         <v>48</v>
@@ -1819,7 +1837,7 @@
         <v>80</v>
       </c>
       <c r="D37" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F37" t="s">
         <v>48</v>
@@ -1845,7 +1863,7 @@
         <v>80</v>
       </c>
       <c r="D38" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F38" t="s">
         <v>48</v>
@@ -1871,7 +1889,7 @@
         <v>80</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F39" t="s">
         <v>48</v>
@@ -1897,7 +1915,7 @@
         <v>80</v>
       </c>
       <c r="D40" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F40" t="s">
         <v>48</v>
@@ -1923,7 +1941,7 @@
         <v>120</v>
       </c>
       <c r="D41" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F41" t="s">
         <v>48</v>
@@ -1949,7 +1967,7 @@
         <v>120</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F42" t="s">
         <v>48</v>
@@ -1975,7 +1993,7 @@
         <v>120</v>
       </c>
       <c r="D43" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F43" t="s">
         <v>48</v>
@@ -2001,7 +2019,7 @@
         <v>120</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F44" t="s">
         <v>48</v>
@@ -2027,7 +2045,7 @@
         <v>120</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F45" t="s">
         <v>48</v>
@@ -2053,7 +2071,7 @@
         <v>60</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F46" t="s">
         <v>82</v>
@@ -2079,7 +2097,7 @@
         <v>60</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F47" t="s">
         <v>82</v>
@@ -2105,7 +2123,7 @@
         <v>60</v>
       </c>
       <c r="D48" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F48" t="s">
         <v>82</v>
@@ -2131,7 +2149,7 @@
         <v>60</v>
       </c>
       <c r="D49" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F49" t="s">
         <v>82</v>
@@ -2157,7 +2175,7 @@
         <v>60</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F50" t="s">
         <v>82</v>
@@ -2183,7 +2201,7 @@
         <v>10</v>
       </c>
       <c r="D51" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F51" t="s">
         <v>82</v>
@@ -2209,7 +2227,7 @@
         <v>10</v>
       </c>
       <c r="D52" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F52" t="s">
         <v>82</v>
@@ -2235,7 +2253,7 @@
         <v>10</v>
       </c>
       <c r="D53" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F53" t="s">
         <v>82</v>
@@ -2261,7 +2279,7 @@
         <v>10</v>
       </c>
       <c r="D54" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F54" t="s">
         <v>82</v>
@@ -2287,7 +2305,7 @@
         <v>10</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F55" t="s">
         <v>82</v>
@@ -2313,7 +2331,7 @@
         <v>30</v>
       </c>
       <c r="D56" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F56" t="s">
         <v>48</v>
@@ -2339,7 +2357,7 @@
         <v>30</v>
       </c>
       <c r="D57" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F57" t="s">
         <v>48</v>
@@ -2365,7 +2383,7 @@
         <v>30</v>
       </c>
       <c r="D58" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F58" t="s">
         <v>48</v>
@@ -2391,7 +2409,7 @@
         <v>30</v>
       </c>
       <c r="D59" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F59" t="s">
         <v>48</v>
@@ -2417,7 +2435,7 @@
         <v>30</v>
       </c>
       <c r="D60" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F60" t="s">
         <v>48</v>
@@ -2443,7 +2461,7 @@
         <v>20</v>
       </c>
       <c r="D61" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F61" t="s">
         <v>48</v>
@@ -2544,7 +2562,7 @@
         <v>60</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F65" s="12" t="s">
         <v>86</v>
@@ -2561,7 +2579,7 @@
     </row>
     <row r="66" spans="1:9">
       <c r="A66" s="15" t="s">
-        <v>91</v>
+        <v>127</v>
       </c>
       <c r="B66" s="16" t="s">
         <v>10</v>
@@ -2587,7 +2605,7 @@
     </row>
     <row r="67" spans="1:9">
       <c r="A67" s="15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B67" s="16" t="s">
         <v>10</v>
@@ -2613,7 +2631,7 @@
     </row>
     <row r="68" spans="1:9">
       <c r="A68" s="15" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B68" s="16" t="s">
         <v>10</v>
@@ -2639,7 +2657,7 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" s="15" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B69" s="16" t="s">
         <v>10</v>
@@ -2665,7 +2683,7 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B70" s="16" t="s">
         <v>10</v>
@@ -2691,7 +2709,7 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B71" s="16" t="s">
         <v>10</v>
@@ -2717,7 +2735,7 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" s="12" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B72" s="16" t="s">
         <v>10</v>
@@ -2743,7 +2761,7 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B73" s="16" t="s">
         <v>10</v>
@@ -2769,7 +2787,7 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B74" s="16" t="s">
         <v>10</v>
@@ -2795,7 +2813,7 @@
     </row>
     <row r="75" spans="1:9">
       <c r="A75" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B75" s="16" t="s">
         <v>10</v>
@@ -2821,7 +2839,7 @@
     </row>
     <row r="76" spans="1:9">
       <c r="A76" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B76" s="16" t="s">
         <v>10</v>
@@ -2847,7 +2865,7 @@
     </row>
     <row r="77" spans="1:9">
       <c r="A77" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B77" s="16" t="s">
         <v>10</v>
@@ -2873,7 +2891,7 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B78" s="16" t="s">
         <v>10</v>
@@ -2899,7 +2917,7 @@
     </row>
     <row r="79" spans="1:9" ht="26.25" customHeight="1">
       <c r="A79" s="10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B79" s="12" t="s">
         <v>10</v>
@@ -2914,7 +2932,7 @@
         <v>14</v>
       </c>
       <c r="G79" s="5">
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="H79">
         <v>4</v>
@@ -2925,7 +2943,7 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B80" s="12" t="s">
         <v>10</v>
@@ -2948,7 +2966,7 @@
     </row>
     <row r="81" spans="1:9">
       <c r="A81" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B81" s="12" t="s">
         <v>10</v>
@@ -2971,7 +2989,7 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B82" s="12" t="s">
         <v>10</v>
@@ -2994,7 +3012,7 @@
     </row>
     <row r="83" spans="1:9">
       <c r="A83" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B83" s="12" t="s">
         <v>10</v>
@@ -3017,7 +3035,7 @@
     </row>
     <row r="84" spans="1:9">
       <c r="A84" s="12" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B84" s="12" t="s">
         <v>10</v>
@@ -3040,7 +3058,7 @@
     </row>
     <row r="85" spans="1:9">
       <c r="A85" s="12" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B85" s="12" t="s">
         <v>10</v>
@@ -3063,7 +3081,7 @@
     </row>
     <row r="86" spans="1:9">
       <c r="A86" s="12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B86" s="12" t="s">
         <v>10</v>
@@ -3086,7 +3104,7 @@
     </row>
     <row r="87" spans="1:9">
       <c r="A87" s="12" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B87" s="12" t="s">
         <v>10</v>
@@ -3109,7 +3127,7 @@
     </row>
     <row r="88" spans="1:9">
       <c r="A88" s="12" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B88" s="12" t="s">
         <v>10</v>
@@ -3132,7 +3150,7 @@
     </row>
     <row r="89" spans="1:9">
       <c r="A89" s="12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B89" s="12" t="s">
         <v>10</v>
@@ -3155,7 +3173,7 @@
     </row>
     <row r="90" spans="1:9">
       <c r="A90" s="12" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B90" s="12" t="s">
         <v>10</v>
@@ -3178,7 +3196,7 @@
     </row>
     <row r="91" spans="1:9">
       <c r="A91" s="12" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B91" s="12" t="s">
         <v>10</v>
@@ -3201,7 +3219,7 @@
     </row>
     <row r="92" spans="1:9">
       <c r="A92" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B92" s="12" t="s">
         <v>10</v>
@@ -3224,7 +3242,7 @@
     </row>
     <row r="93" spans="1:9">
       <c r="A93" s="12" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B93" s="12" t="s">
         <v>10</v>
@@ -3247,7 +3265,7 @@
     </row>
     <row r="94" spans="1:9">
       <c r="A94" s="12" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B94" s="12" t="s">
         <v>10</v>
@@ -3270,7 +3288,7 @@
     </row>
     <row r="95" spans="1:9">
       <c r="A95" s="12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B95" s="12" t="s">
         <v>10</v>
@@ -3293,7 +3311,7 @@
     </row>
     <row r="96" spans="1:9">
       <c r="A96" s="17" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B96" s="12" t="s">
         <v>10</v>
@@ -3310,13 +3328,13 @@
       <c r="G96" s="5">
         <v>2</v>
       </c>
-      <c r="I96" s="7" t="s">
+      <c r="I96" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="97" spans="1:9">
       <c r="A97" s="17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B97" s="12" t="s">
         <v>10</v>
@@ -3333,13 +3351,13 @@
       <c r="G97" s="5">
         <v>2</v>
       </c>
-      <c r="I97" s="20" t="s">
+      <c r="I97" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="98" spans="1:9">
       <c r="A98" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B98" s="12" t="s">
         <v>10</v>
@@ -3356,13 +3374,13 @@
       <c r="G98" s="5">
         <v>2</v>
       </c>
-      <c r="I98" s="7" t="s">
+      <c r="I98" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="99" spans="1:9">
       <c r="A99" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B99" s="12" t="s">
         <v>10</v>
@@ -3379,13 +3397,13 @@
       <c r="G99" s="5">
         <v>2</v>
       </c>
-      <c r="I99" s="20" t="s">
+      <c r="I99" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="100" spans="1:9">
       <c r="A100" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B100" s="12" t="s">
         <v>10</v>
@@ -3402,13 +3420,13 @@
       <c r="G100" s="5">
         <v>2</v>
       </c>
-      <c r="I100" s="7" t="s">
+      <c r="I100" s="20" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="101" spans="1:9">
       <c r="A101" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B101" s="12" t="s">
         <v>10</v>
@@ -3430,10 +3448,142 @@
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="G102" s="5"/>
+      <c r="A102" s="15" t="s">
+        <v>128</v>
+      </c>
+      <c r="B102" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C102">
+        <v>30</v>
+      </c>
+      <c r="D102" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F102" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G102" s="5">
+        <v>2</v>
+      </c>
+      <c r="I102" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="103" spans="1:9">
-      <c r="G103" s="5"/>
+      <c r="A103" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B103" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C103">
+        <v>30</v>
+      </c>
+      <c r="D103" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F103" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G103" s="5">
+        <v>2</v>
+      </c>
+      <c r="I103" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" s="15" t="s">
+        <v>130</v>
+      </c>
+      <c r="B104" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C104">
+        <v>30</v>
+      </c>
+      <c r="D104" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F104" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G104" s="5">
+        <v>2</v>
+      </c>
+      <c r="I104" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="B105" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C105">
+        <v>30</v>
+      </c>
+      <c r="D105" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F105" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G105" s="5">
+        <v>2</v>
+      </c>
+      <c r="I105" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" s="15" t="s">
+        <v>132</v>
+      </c>
+      <c r="B106" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C106">
+        <v>30</v>
+      </c>
+      <c r="D106" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F106" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G106" s="5">
+        <v>2</v>
+      </c>
+      <c r="I106" s="20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" s="15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B107" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C107">
+        <v>30</v>
+      </c>
+      <c r="D107" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="F107" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="G107" s="5">
+        <v>2</v>
+      </c>
+      <c r="I107" s="7" t="s">
+        <v>31</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>
@@ -3499,22 +3649,28 @@
     <hyperlink ref="I90" r:id="rId59"/>
     <hyperlink ref="I92" r:id="rId60"/>
     <hyperlink ref="I94" r:id="rId61"/>
-    <hyperlink ref="I96" r:id="rId62"/>
-    <hyperlink ref="I98" r:id="rId63"/>
-    <hyperlink ref="I100" r:id="rId64"/>
-    <hyperlink ref="I83" r:id="rId65"/>
-    <hyperlink ref="I85" r:id="rId66"/>
-    <hyperlink ref="I87" r:id="rId67"/>
-    <hyperlink ref="I89" r:id="rId68"/>
-    <hyperlink ref="I91" r:id="rId69"/>
-    <hyperlink ref="I93" r:id="rId70"/>
-    <hyperlink ref="I95" r:id="rId71"/>
-    <hyperlink ref="I97" r:id="rId72"/>
-    <hyperlink ref="I99" r:id="rId73"/>
-    <hyperlink ref="I101" r:id="rId74"/>
+    <hyperlink ref="I83" r:id="rId62"/>
+    <hyperlink ref="I85" r:id="rId63"/>
+    <hyperlink ref="I87" r:id="rId64"/>
+    <hyperlink ref="I89" r:id="rId65"/>
+    <hyperlink ref="I91" r:id="rId66"/>
+    <hyperlink ref="I93" r:id="rId67"/>
+    <hyperlink ref="I95" r:id="rId68"/>
+    <hyperlink ref="I97" r:id="rId69"/>
+    <hyperlink ref="I102" r:id="rId70"/>
+    <hyperlink ref="I107" r:id="rId71"/>
+    <hyperlink ref="I99" r:id="rId72"/>
+    <hyperlink ref="I104" r:id="rId73"/>
+    <hyperlink ref="I96" r:id="rId74"/>
+    <hyperlink ref="I101" r:id="rId75"/>
+    <hyperlink ref="I106" r:id="rId76"/>
+    <hyperlink ref="I98" r:id="rId77"/>
+    <hyperlink ref="I103" r:id="rId78"/>
+    <hyperlink ref="I100" r:id="rId79"/>
+    <hyperlink ref="I105" r:id="rId80"/>
   </hyperlinks>
   <pageMargins left="0.78740157499999996" right="0.78740157499999996" top="0.984251969" bottom="0.984251969" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId75"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId81"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Nova Espec. Caso de Uso Configuração das portas
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="555" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="557" uniqueCount="136">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -418,6 +418,12 @@
   </si>
   <si>
     <t>Criar Planilha de Caso de Teste Cad. Auxiliar_Tipo de Manutenção</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.45</t>
   </si>
 </sst>
 </file>
@@ -871,8 +877,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="90" workbookViewId="0">
-      <selection activeCell="A113" sqref="A113"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2596,8 +2602,8 @@
       <c r="G66" s="5">
         <v>1</v>
       </c>
-      <c r="H66">
-        <v>0</v>
+      <c r="H66" t="s">
+        <v>134</v>
       </c>
       <c r="I66" s="7" t="s">
         <v>31</v>
@@ -2622,8 +2628,8 @@
       <c r="G67" s="5">
         <v>1</v>
       </c>
-      <c r="H67">
-        <v>0</v>
+      <c r="H67" t="s">
+        <v>135</v>
       </c>
       <c r="I67" s="7" t="s">
         <v>31</v>
@@ -2935,7 +2941,7 @@
         <v>128</v>
       </c>
       <c r="H79">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I79" s="7" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Liberação da versão Demo do S-Track
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="140">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -427,6 +427,15 @@
   </si>
   <si>
     <t xml:space="preserve">                     0.11</t>
+  </si>
+  <si>
+    <t>Liberação de versão "Demonstração" do S-Track</t>
+  </si>
+  <si>
+    <t>Compelto</t>
+  </si>
+  <si>
+    <t>http://189.126.110.196/demo/</t>
   </si>
 </sst>
 </file>
@@ -538,7 +547,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -582,6 +591,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -878,10 +890,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="90" workbookViewId="0">
-      <selection activeCell="J66" sqref="J66"/>
+    <sheetView tabSelected="1" topLeftCell="C85" zoomScale="90" workbookViewId="0">
+      <selection activeCell="I112" sqref="I112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -3592,6 +3604,32 @@
       </c>
       <c r="I107" s="7" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" s="21" t="s">
+        <v>137</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C108">
+        <v>50</v>
+      </c>
+      <c r="D108" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="F108" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G108" s="5">
+        <v>24</v>
+      </c>
+      <c r="H108">
+        <v>18</v>
+      </c>
+      <c r="I108" t="s">
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Especif. caso uso e cadastro rastreador no sistema
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="142">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -436,6 +436,12 @@
   </si>
   <si>
     <t>http://189.126.110.196/demo/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.18</t>
   </si>
 </sst>
 </file>
@@ -893,8 +899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B77" zoomScale="90" workbookViewId="0">
-      <selection activeCell="I108" sqref="I108"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H68" sqref="H68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2671,7 +2677,7 @@
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>31</v>
@@ -2697,7 +2703,7 @@
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Conclusão Especf. Caso de Uso
</commit_message>
<xml_diff>
--- a/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
+++ b/Acompanhamento/Work_Items_list_Sistema de Rastreamento.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="573" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="150">
   <si>
     <t>Nome / Descrição</t>
   </si>
@@ -426,9 +426,6 @@
     <t xml:space="preserve">                     0.45</t>
   </si>
   <si>
-    <t xml:space="preserve">                     0.11</t>
-  </si>
-  <si>
     <t>Liberação de versão "Demonstração" do S-Track</t>
   </si>
   <si>
@@ -442,6 +439,33 @@
   </si>
   <si>
     <t xml:space="preserve">                     0.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                     0.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       2.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                       2.6</t>
   </si>
 </sst>
 </file>
@@ -553,7 +577,7 @@
     <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -601,6 +625,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -899,8 +924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I108"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="90" workbookViewId="0">
-      <selection activeCell="H68" sqref="H68"/>
+    <sheetView tabSelected="1" topLeftCell="A71" zoomScale="90" workbookViewId="0">
+      <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2616,7 +2641,7 @@
         <v>60</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F66" s="12" t="s">
         <v>86</v>
@@ -2642,7 +2667,7 @@
         <v>60</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F67" s="12" t="s">
         <v>86</v>
@@ -2668,7 +2693,7 @@
         <v>60</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F68" s="12" t="s">
         <v>86</v>
@@ -2677,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="H68" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I68" s="7" t="s">
         <v>31</v>
@@ -2694,7 +2719,7 @@
         <v>60</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F69" s="12" t="s">
         <v>86</v>
@@ -2703,7 +2728,7 @@
         <v>1</v>
       </c>
       <c r="H69" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I69" s="7" t="s">
         <v>31</v>
@@ -2720,7 +2745,7 @@
         <v>60</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F70" s="12" t="s">
         <v>86</v>
@@ -2728,8 +2753,8 @@
       <c r="G70" s="5">
         <v>1</v>
       </c>
-      <c r="H70" t="s">
-        <v>136</v>
+      <c r="H70" s="23" t="s">
+        <v>141</v>
       </c>
       <c r="I70" s="7" t="s">
         <v>31</v>
@@ -2746,7 +2771,7 @@
         <v>60</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F71" s="12" t="s">
         <v>86</v>
@@ -2754,8 +2779,8 @@
       <c r="G71" s="5">
         <v>1</v>
       </c>
-      <c r="H71" t="s">
-        <v>136</v>
+      <c r="H71" s="23" t="s">
+        <v>139</v>
       </c>
       <c r="I71" s="7" t="s">
         <v>31</v>
@@ -2772,7 +2797,7 @@
         <v>60</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F72" s="12" t="s">
         <v>86</v>
@@ -2780,8 +2805,8 @@
       <c r="G72" s="5">
         <v>1</v>
       </c>
-      <c r="H72" t="s">
-        <v>136</v>
+      <c r="H72" s="23" t="s">
+        <v>142</v>
       </c>
       <c r="I72" s="7" t="s">
         <v>31</v>
@@ -2798,7 +2823,7 @@
         <v>60</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F73" s="12" t="s">
         <v>86</v>
@@ -2806,8 +2831,8 @@
       <c r="G73" s="5">
         <v>1</v>
       </c>
-      <c r="H73" t="s">
-        <v>136</v>
+      <c r="H73" s="23" t="s">
+        <v>140</v>
       </c>
       <c r="I73" s="7" t="s">
         <v>31</v>
@@ -2824,7 +2849,7 @@
         <v>60</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F74" s="12" t="s">
         <v>86</v>
@@ -2832,8 +2857,8 @@
       <c r="G74" s="5">
         <v>1</v>
       </c>
-      <c r="H74" t="s">
-        <v>136</v>
+      <c r="H74" s="23" t="s">
+        <v>143</v>
       </c>
       <c r="I74" s="7" t="s">
         <v>31</v>
@@ -2850,7 +2875,7 @@
         <v>60</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F75" s="12" t="s">
         <v>86</v>
@@ -2858,8 +2883,8 @@
       <c r="G75" s="5">
         <v>1</v>
       </c>
-      <c r="H75" t="s">
-        <v>136</v>
+      <c r="H75" s="23" t="s">
+        <v>144</v>
       </c>
       <c r="I75" s="7" t="s">
         <v>31</v>
@@ -2876,7 +2901,7 @@
         <v>60</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F76" s="12" t="s">
         <v>86</v>
@@ -2884,8 +2909,8 @@
       <c r="G76" s="5">
         <v>1</v>
       </c>
-      <c r="H76" t="s">
-        <v>136</v>
+      <c r="H76" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="I76" s="7" t="s">
         <v>31</v>
@@ -2902,7 +2927,7 @@
         <v>60</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F77" s="12" t="s">
         <v>86</v>
@@ -2910,8 +2935,8 @@
       <c r="G77" s="5">
         <v>1</v>
       </c>
-      <c r="H77" t="s">
-        <v>136</v>
+      <c r="H77" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="I77" s="7" t="s">
         <v>31</v>
@@ -2928,7 +2953,7 @@
         <v>60</v>
       </c>
       <c r="D78" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F78" s="12" t="s">
         <v>86</v>
@@ -2936,8 +2961,8 @@
       <c r="G78" s="5">
         <v>1</v>
       </c>
-      <c r="H78" t="s">
-        <v>136</v>
+      <c r="H78" s="23" t="s">
+        <v>145</v>
       </c>
       <c r="I78" s="7" t="s">
         <v>31</v>
@@ -2954,7 +2979,7 @@
         <v>440</v>
       </c>
       <c r="D79" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F79" t="s">
         <v>14</v>
@@ -2980,13 +3005,16 @@
         <v>50</v>
       </c>
       <c r="D80" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F80" t="s">
         <v>14</v>
       </c>
       <c r="G80" s="5">
         <v>4</v>
+      </c>
+      <c r="H80">
+        <v>2</v>
       </c>
       <c r="I80" s="7" t="s">
         <v>31</v>
@@ -3003,13 +3031,16 @@
         <v>50</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F81" t="s">
         <v>14</v>
       </c>
       <c r="G81" s="5">
         <v>4</v>
+      </c>
+      <c r="H81" t="s">
+        <v>146</v>
       </c>
       <c r="I81" s="20" t="s">
         <v>31</v>
@@ -3026,13 +3057,16 @@
         <v>50</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F82" t="s">
         <v>14</v>
       </c>
       <c r="G82" s="5">
         <v>4</v>
+      </c>
+      <c r="H82" t="s">
+        <v>147</v>
       </c>
       <c r="I82" s="7" t="s">
         <v>31</v>
@@ -3049,13 +3083,16 @@
         <v>50</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F83" t="s">
         <v>14</v>
       </c>
       <c r="G83" s="5">
         <v>4</v>
+      </c>
+      <c r="H83">
+        <v>2</v>
       </c>
       <c r="I83" s="20" t="s">
         <v>31</v>
@@ -3072,13 +3109,16 @@
         <v>50</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F84" t="s">
         <v>14</v>
       </c>
       <c r="G84" s="5">
         <v>4</v>
+      </c>
+      <c r="H84" t="s">
+        <v>146</v>
       </c>
       <c r="I84" s="7" t="s">
         <v>31</v>
@@ -3095,13 +3135,16 @@
         <v>50</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F85" t="s">
         <v>14</v>
       </c>
       <c r="G85" s="5">
         <v>4</v>
+      </c>
+      <c r="H85" t="s">
+        <v>147</v>
       </c>
       <c r="I85" s="20" t="s">
         <v>31</v>
@@ -3118,13 +3161,16 @@
         <v>50</v>
       </c>
       <c r="D86" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F86" t="s">
         <v>14</v>
       </c>
       <c r="G86" s="5">
         <v>4</v>
+      </c>
+      <c r="H86">
+        <v>2</v>
       </c>
       <c r="I86" s="7" t="s">
         <v>31</v>
@@ -3141,13 +3187,16 @@
         <v>50</v>
       </c>
       <c r="D87" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F87" t="s">
         <v>14</v>
       </c>
       <c r="G87" s="5">
         <v>4</v>
+      </c>
+      <c r="H87" t="s">
+        <v>148</v>
       </c>
       <c r="I87" s="20" t="s">
         <v>31</v>
@@ -3164,13 +3213,16 @@
         <v>50</v>
       </c>
       <c r="D88" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F88" t="s">
         <v>14</v>
       </c>
       <c r="G88" s="5">
         <v>4</v>
+      </c>
+      <c r="H88">
+        <v>2</v>
       </c>
       <c r="I88" s="7" t="s">
         <v>31</v>
@@ -3187,13 +3239,16 @@
         <v>50</v>
       </c>
       <c r="D89" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F89" t="s">
         <v>14</v>
       </c>
       <c r="G89" s="5">
         <v>4</v>
+      </c>
+      <c r="H89">
+        <v>3</v>
       </c>
       <c r="I89" s="20" t="s">
         <v>31</v>
@@ -3210,13 +3265,16 @@
         <v>50</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F90" t="s">
         <v>14</v>
       </c>
       <c r="G90" s="5">
         <v>4</v>
+      </c>
+      <c r="H90">
+        <v>2</v>
       </c>
       <c r="I90" s="7" t="s">
         <v>31</v>
@@ -3233,13 +3291,16 @@
         <v>50</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F91" t="s">
         <v>14</v>
       </c>
       <c r="G91" s="5">
         <v>4</v>
+      </c>
+      <c r="H91" t="s">
+        <v>148</v>
       </c>
       <c r="I91" s="20" t="s">
         <v>31</v>
@@ -3256,13 +3317,16 @@
         <v>50</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F92" t="s">
         <v>14</v>
       </c>
       <c r="G92" s="5">
         <v>4</v>
+      </c>
+      <c r="H92" t="s">
+        <v>149</v>
       </c>
       <c r="I92" s="7" t="s">
         <v>31</v>
@@ -3279,13 +3343,16 @@
         <v>50</v>
       </c>
       <c r="D93" s="11" t="s">
-        <v>88</v>
+        <v>104</v>
       </c>
       <c r="F93" t="s">
         <v>14</v>
       </c>
       <c r="G93" s="5">
         <v>4</v>
+      </c>
+      <c r="H93">
+        <v>2</v>
       </c>
       <c r="I93" s="20" t="s">
         <v>31</v>
@@ -3310,6 +3377,9 @@
       <c r="G94" s="5">
         <v>3.5</v>
       </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
       <c r="I94" s="7" t="s">
         <v>31</v>
       </c>
@@ -3615,7 +3685,7 @@
     </row>
     <row r="108" spans="1:9">
       <c r="A108" s="21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B108" s="12" t="s">
         <v>9</v>
@@ -3624,7 +3694,7 @@
         <v>50</v>
       </c>
       <c r="D108" s="11" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F108" s="12" t="s">
         <v>86</v>
@@ -3636,7 +3706,7 @@
         <v>18</v>
       </c>
       <c r="I108" s="22" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>